<commit_message>
Adding updated TotalExercise file
</commit_message>
<xml_diff>
--- a/datasets/TotalExercise.xlsx
+++ b/datasets/TotalExercise.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="TotalExercise" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -908,8 +908,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O92"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Adding Jan 2018 TotalExercies numbers
</commit_message>
<xml_diff>
--- a/datasets/TotalExercise.xlsx
+++ b/datasets/TotalExercise.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -552,11 +552,12 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -913,10 +914,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O123"/>
+  <dimension ref="A1:O154"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O109" sqref="O109:O123"/>
+      <selection activeCell="O123" sqref="O123:O154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4394,19 +4395,19 @@
         <v>1436</v>
       </c>
       <c r="K67" t="str">
-        <f t="shared" ref="K67:K123" si="5">IF(C67&gt;8000,"Yes","No")</f>
+        <f t="shared" ref="K67:K130" si="5">IF(C67&gt;8000,"Yes","No")</f>
         <v>No</v>
       </c>
       <c r="L67" t="str">
-        <f t="shared" ref="L67:L123" si="6">IF(B67&gt;3400,"Yes","No")</f>
+        <f t="shared" ref="L67:L130" si="6">IF(B67&gt;3400,"Yes","No")</f>
         <v>No</v>
       </c>
       <c r="M67" t="str">
-        <f t="shared" ref="M67:M123" si="7">IF(I67&gt;30,"Yes","No")</f>
+        <f t="shared" ref="M67:M130" si="7">IF(I67&gt;30,"Yes","No")</f>
         <v>No</v>
       </c>
       <c r="N67" t="str">
-        <f t="shared" ref="N67:N123" si="8">IF(I67+H67&lt;30,"Yes","No")</f>
+        <f t="shared" ref="N67:N130" si="8">IF(I67+H67&lt;30,"Yes","No")</f>
         <v>No</v>
       </c>
       <c r="O67" t="str">
@@ -5710,7 +5711,7 @@
         <v>No</v>
       </c>
       <c r="O92" t="str">
-        <f>IF(D92&gt;5,"Yes","No")</f>
+        <f t="shared" ref="O92:O109" si="10">IF(D92&gt;5,"Yes","No")</f>
         <v>Yes</v>
       </c>
     </row>
@@ -5762,7 +5763,7 @@
         <v>No</v>
       </c>
       <c r="O93" t="str">
-        <f>IF(D93&gt;5,"Yes","No")</f>
+        <f t="shared" si="10"/>
         <v>Yes</v>
       </c>
     </row>
@@ -5814,7 +5815,7 @@
         <v>Yes</v>
       </c>
       <c r="O94" t="str">
-        <f>IF(D94&gt;5,"Yes","No")</f>
+        <f t="shared" si="10"/>
         <v>Yes</v>
       </c>
     </row>
@@ -5866,7 +5867,7 @@
         <v>No</v>
       </c>
       <c r="O95" t="str">
-        <f>IF(D95&gt;5,"Yes","No")</f>
+        <f t="shared" si="10"/>
         <v>Yes</v>
       </c>
     </row>
@@ -5918,7 +5919,7 @@
         <v>No</v>
       </c>
       <c r="O96" t="str">
-        <f>IF(D96&gt;5,"Yes","No")</f>
+        <f t="shared" si="10"/>
         <v>Yes</v>
       </c>
     </row>
@@ -5970,7 +5971,7 @@
         <v>Yes</v>
       </c>
       <c r="O97" t="str">
-        <f>IF(D97&gt;5,"Yes","No")</f>
+        <f t="shared" si="10"/>
         <v>Yes</v>
       </c>
     </row>
@@ -6022,7 +6023,7 @@
         <v>No</v>
       </c>
       <c r="O98" t="str">
-        <f>IF(D98&gt;5,"Yes","No")</f>
+        <f t="shared" si="10"/>
         <v>Yes</v>
       </c>
     </row>
@@ -6074,7 +6075,7 @@
         <v>No</v>
       </c>
       <c r="O99" t="str">
-        <f>IF(D99&gt;5,"Yes","No")</f>
+        <f t="shared" si="10"/>
         <v>Yes</v>
       </c>
     </row>
@@ -6126,7 +6127,7 @@
         <v>Yes</v>
       </c>
       <c r="O100" t="str">
-        <f>IF(D100&gt;5,"Yes","No")</f>
+        <f t="shared" si="10"/>
         <v>Yes</v>
       </c>
     </row>
@@ -6178,7 +6179,7 @@
         <v>No</v>
       </c>
       <c r="O101" t="str">
-        <f>IF(D101&gt;5,"Yes","No")</f>
+        <f t="shared" si="10"/>
         <v>Yes</v>
       </c>
     </row>
@@ -6230,7 +6231,7 @@
         <v>Yes</v>
       </c>
       <c r="O102" t="str">
-        <f>IF(D102&gt;5,"Yes","No")</f>
+        <f t="shared" si="10"/>
         <v>Yes</v>
       </c>
     </row>
@@ -6282,7 +6283,7 @@
         <v>No</v>
       </c>
       <c r="O103" t="str">
-        <f>IF(D103&gt;5,"Yes","No")</f>
+        <f t="shared" si="10"/>
         <v>Yes</v>
       </c>
     </row>
@@ -6334,7 +6335,7 @@
         <v>No</v>
       </c>
       <c r="O104" t="str">
-        <f>IF(D104&gt;5,"Yes","No")</f>
+        <f t="shared" si="10"/>
         <v>Yes</v>
       </c>
     </row>
@@ -6386,7 +6387,7 @@
         <v>Yes</v>
       </c>
       <c r="O105" t="str">
-        <f>IF(D105&gt;5,"Yes","No")</f>
+        <f t="shared" si="10"/>
         <v>No</v>
       </c>
     </row>
@@ -6438,7 +6439,7 @@
         <v>No</v>
       </c>
       <c r="O106" t="str">
-        <f>IF(D106&gt;5,"Yes","No")</f>
+        <f t="shared" si="10"/>
         <v>Yes</v>
       </c>
     </row>
@@ -6490,7 +6491,7 @@
         <v>Yes</v>
       </c>
       <c r="O107" t="str">
-        <f>IF(D107&gt;5,"Yes","No")</f>
+        <f t="shared" si="10"/>
         <v>No</v>
       </c>
     </row>
@@ -6542,7 +6543,7 @@
         <v>Yes</v>
       </c>
       <c r="O108" t="str">
-        <f>IF(D108&gt;5,"Yes","No")</f>
+        <f t="shared" si="10"/>
         <v>No</v>
       </c>
     </row>
@@ -6594,7 +6595,7 @@
         <v>Yes</v>
       </c>
       <c r="O109" t="str">
-        <f>IF(D109&gt;5,"Yes","No")</f>
+        <f t="shared" si="10"/>
         <v>No</v>
       </c>
     </row>
@@ -6646,7 +6647,7 @@
         <v>Yes</v>
       </c>
       <c r="O110" t="str">
-        <f t="shared" ref="O110:O123" si="10">IF(D110&gt;5,"Yes","No")</f>
+        <f t="shared" ref="O110:O154" si="11">IF(D110&gt;5,"Yes","No")</f>
         <v>No</v>
       </c>
     </row>
@@ -6698,7 +6699,7 @@
         <v>Yes</v>
       </c>
       <c r="O111" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>Yes</v>
       </c>
     </row>
@@ -6750,7 +6751,7 @@
         <v>No</v>
       </c>
       <c r="O112" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>Yes</v>
       </c>
     </row>
@@ -6802,7 +6803,7 @@
         <v>No</v>
       </c>
       <c r="O113" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>Yes</v>
       </c>
     </row>
@@ -6854,7 +6855,7 @@
         <v>Yes</v>
       </c>
       <c r="O114" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>Yes</v>
       </c>
     </row>
@@ -6906,7 +6907,7 @@
         <v>No</v>
       </c>
       <c r="O115" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>Yes</v>
       </c>
     </row>
@@ -6958,7 +6959,7 @@
         <v>No</v>
       </c>
       <c r="O116" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>Yes</v>
       </c>
     </row>
@@ -7010,7 +7011,7 @@
         <v>Yes</v>
       </c>
       <c r="O117" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>No</v>
       </c>
     </row>
@@ -7062,7 +7063,7 @@
         <v>Yes</v>
       </c>
       <c r="O118" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>Yes</v>
       </c>
     </row>
@@ -7114,7 +7115,7 @@
         <v>No</v>
       </c>
       <c r="O119" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>Yes</v>
       </c>
     </row>
@@ -7166,7 +7167,7 @@
         <v>No</v>
       </c>
       <c r="O120" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>Yes</v>
       </c>
     </row>
@@ -7218,7 +7219,7 @@
         <v>No</v>
       </c>
       <c r="O121" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>Yes</v>
       </c>
     </row>
@@ -7270,7 +7271,7 @@
         <v>Yes</v>
       </c>
       <c r="O122" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>Yes</v>
       </c>
     </row>
@@ -7322,7 +7323,1619 @@
         <v>Yes</v>
       </c>
       <c r="O123" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="124" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A124" s="1">
+        <v>43101</v>
+      </c>
+      <c r="B124" s="2">
+        <v>3006</v>
+      </c>
+      <c r="C124" s="2">
+        <v>6574</v>
+      </c>
+      <c r="D124" s="3">
+        <v>5.1100000000000003</v>
+      </c>
+      <c r="E124" s="2">
+        <v>0</v>
+      </c>
+      <c r="F124">
+        <v>699</v>
+      </c>
+      <c r="G124">
+        <v>295</v>
+      </c>
+      <c r="H124" s="2">
+        <v>0</v>
+      </c>
+      <c r="I124" s="2">
+        <v>0</v>
+      </c>
+      <c r="J124" s="2">
+        <v>1265</v>
+      </c>
+      <c r="K124" t="str">
+        <f t="shared" si="5"/>
+        <v>No</v>
+      </c>
+      <c r="L124" t="str">
+        <f t="shared" si="6"/>
+        <v>No</v>
+      </c>
+      <c r="M124" t="str">
+        <f t="shared" si="7"/>
+        <v>No</v>
+      </c>
+      <c r="N124" t="str">
+        <f t="shared" si="8"/>
+        <v>Yes</v>
+      </c>
+      <c r="O124" t="str">
+        <f t="shared" si="11"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="125" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A125" s="1">
+        <v>43102</v>
+      </c>
+      <c r="B125" s="2">
+        <v>3262</v>
+      </c>
+      <c r="C125" s="2">
+        <v>8239</v>
+      </c>
+      <c r="D125" s="3">
+        <v>6.43</v>
+      </c>
+      <c r="E125" s="2">
+        <v>16</v>
+      </c>
+      <c r="F125">
+        <v>812</v>
+      </c>
+      <c r="G125">
+        <v>312</v>
+      </c>
+      <c r="H125" s="2">
+        <v>0</v>
+      </c>
+      <c r="I125" s="2">
+        <v>0</v>
+      </c>
+      <c r="J125" s="2">
+        <v>1485</v>
+      </c>
+      <c r="K125" t="str">
+        <f t="shared" si="5"/>
+        <v>Yes</v>
+      </c>
+      <c r="L125" t="str">
+        <f t="shared" si="6"/>
+        <v>No</v>
+      </c>
+      <c r="M125" t="str">
+        <f t="shared" si="7"/>
+        <v>No</v>
+      </c>
+      <c r="N125" t="str">
+        <f t="shared" si="8"/>
+        <v>Yes</v>
+      </c>
+      <c r="O125" t="str">
+        <f t="shared" si="11"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="126" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A126" s="1">
+        <v>43103</v>
+      </c>
+      <c r="B126" s="2">
+        <v>3372</v>
+      </c>
+      <c r="C126" s="2">
+        <v>6634</v>
+      </c>
+      <c r="D126" s="3">
+        <v>5.17</v>
+      </c>
+      <c r="E126" s="2">
+        <v>23</v>
+      </c>
+      <c r="F126">
+        <v>658</v>
+      </c>
+      <c r="G126">
+        <v>268</v>
+      </c>
+      <c r="H126" s="2">
+        <v>0</v>
+      </c>
+      <c r="I126" s="2">
+        <v>0</v>
+      </c>
+      <c r="J126" s="2">
+        <v>1403</v>
+      </c>
+      <c r="K126" t="str">
+        <f t="shared" si="5"/>
+        <v>No</v>
+      </c>
+      <c r="L126" t="str">
+        <f t="shared" si="6"/>
+        <v>No</v>
+      </c>
+      <c r="M126" t="str">
+        <f t="shared" si="7"/>
+        <v>No</v>
+      </c>
+      <c r="N126" t="str">
+        <f t="shared" si="8"/>
+        <v>Yes</v>
+      </c>
+      <c r="O126" t="str">
+        <f t="shared" si="11"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="127" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A127" s="1">
+        <v>43104</v>
+      </c>
+      <c r="B127" s="2">
+        <v>3765</v>
+      </c>
+      <c r="C127" s="2">
+        <v>15038</v>
+      </c>
+      <c r="D127" s="3">
+        <v>11.73</v>
+      </c>
+      <c r="E127" s="2">
+        <v>4</v>
+      </c>
+      <c r="F127">
+        <v>582</v>
+      </c>
+      <c r="G127">
+        <v>228</v>
+      </c>
+      <c r="H127" s="2">
+        <v>29</v>
+      </c>
+      <c r="I127" s="2">
+        <v>67</v>
+      </c>
+      <c r="J127" s="2">
+        <v>1943</v>
+      </c>
+      <c r="K127" t="str">
+        <f t="shared" si="5"/>
+        <v>Yes</v>
+      </c>
+      <c r="L127" t="str">
+        <f t="shared" si="6"/>
+        <v>Yes</v>
+      </c>
+      <c r="M127" t="str">
+        <f t="shared" si="7"/>
+        <v>Yes</v>
+      </c>
+      <c r="N127" t="str">
+        <f t="shared" si="8"/>
+        <v>No</v>
+      </c>
+      <c r="O127" t="str">
+        <f t="shared" si="11"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="128" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A128" s="1">
+        <v>43105</v>
+      </c>
+      <c r="B128" s="2">
+        <v>3195</v>
+      </c>
+      <c r="C128" s="2">
+        <v>7481</v>
+      </c>
+      <c r="D128" s="3">
+        <v>5.84</v>
+      </c>
+      <c r="E128" s="2">
+        <v>9</v>
+      </c>
+      <c r="F128">
+        <v>699</v>
+      </c>
+      <c r="G128">
+        <v>229</v>
+      </c>
+      <c r="H128" s="2">
+        <v>19</v>
+      </c>
+      <c r="I128" s="2">
+        <v>0</v>
+      </c>
+      <c r="J128" s="2">
+        <v>1212</v>
+      </c>
+      <c r="K128" t="str">
+        <f t="shared" si="5"/>
+        <v>No</v>
+      </c>
+      <c r="L128" t="str">
+        <f t="shared" si="6"/>
+        <v>No</v>
+      </c>
+      <c r="M128" t="str">
+        <f t="shared" si="7"/>
+        <v>No</v>
+      </c>
+      <c r="N128" t="str">
+        <f t="shared" si="8"/>
+        <v>Yes</v>
+      </c>
+      <c r="O128" t="str">
+        <f t="shared" si="11"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="129" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A129" s="1">
+        <v>43106</v>
+      </c>
+      <c r="B129" s="2">
+        <v>3870</v>
+      </c>
+      <c r="C129" s="2">
+        <v>10504</v>
+      </c>
+      <c r="D129" s="3">
+        <v>7.8</v>
+      </c>
+      <c r="E129" s="2">
+        <v>10</v>
+      </c>
+      <c r="F129">
+        <v>685</v>
+      </c>
+      <c r="G129">
+        <v>289</v>
+      </c>
+      <c r="H129" s="2">
+        <v>37</v>
+      </c>
+      <c r="I129" s="2">
+        <v>58</v>
+      </c>
+      <c r="J129" s="2">
+        <v>2253</v>
+      </c>
+      <c r="K129" t="str">
+        <f t="shared" si="5"/>
+        <v>Yes</v>
+      </c>
+      <c r="L129" t="str">
+        <f t="shared" si="6"/>
+        <v>Yes</v>
+      </c>
+      <c r="M129" t="str">
+        <f t="shared" si="7"/>
+        <v>Yes</v>
+      </c>
+      <c r="N129" t="str">
+        <f t="shared" si="8"/>
+        <v>No</v>
+      </c>
+      <c r="O129" t="str">
+        <f t="shared" si="11"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="130" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A130" s="1">
+        <v>43107</v>
+      </c>
+      <c r="B130" s="2">
+        <v>3795</v>
+      </c>
+      <c r="C130" s="2">
+        <v>9245</v>
+      </c>
+      <c r="D130" s="3">
+        <v>6.93</v>
+      </c>
+      <c r="E130" s="2">
+        <v>14</v>
+      </c>
+      <c r="F130">
+        <v>552</v>
+      </c>
+      <c r="G130">
+        <v>298</v>
+      </c>
+      <c r="H130" s="2">
+        <v>28</v>
+      </c>
+      <c r="I130" s="2">
+        <v>40</v>
+      </c>
+      <c r="J130" s="2">
+        <v>2105</v>
+      </c>
+      <c r="K130" t="str">
+        <f t="shared" si="5"/>
+        <v>Yes</v>
+      </c>
+      <c r="L130" t="str">
+        <f t="shared" si="6"/>
+        <v>Yes</v>
+      </c>
+      <c r="M130" t="str">
+        <f t="shared" si="7"/>
+        <v>Yes</v>
+      </c>
+      <c r="N130" t="str">
+        <f t="shared" si="8"/>
+        <v>No</v>
+      </c>
+      <c r="O130" t="str">
+        <f t="shared" si="11"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="131" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A131" s="1">
+        <v>43108</v>
+      </c>
+      <c r="B131" s="2">
+        <v>3674</v>
+      </c>
+      <c r="C131" s="2">
+        <v>10130</v>
+      </c>
+      <c r="D131" s="3">
+        <v>7.64</v>
+      </c>
+      <c r="E131" s="2">
+        <v>9</v>
+      </c>
+      <c r="F131">
+        <v>738</v>
+      </c>
+      <c r="G131">
+        <v>282</v>
+      </c>
+      <c r="H131" s="2">
+        <v>16</v>
+      </c>
+      <c r="I131" s="2">
+        <v>54</v>
+      </c>
+      <c r="J131" s="2">
+        <v>2017</v>
+      </c>
+      <c r="K131" t="str">
+        <f t="shared" ref="K131:K154" si="12">IF(C131&gt;8000,"Yes","No")</f>
+        <v>Yes</v>
+      </c>
+      <c r="L131" t="str">
+        <f t="shared" ref="L131:L154" si="13">IF(B131&gt;3400,"Yes","No")</f>
+        <v>Yes</v>
+      </c>
+      <c r="M131" t="str">
+        <f t="shared" ref="M131:M154" si="14">IF(I131&gt;30,"Yes","No")</f>
+        <v>Yes</v>
+      </c>
+      <c r="N131" t="str">
+        <f t="shared" ref="N131:N154" si="15">IF(I131+H131&lt;30,"Yes","No")</f>
+        <v>No</v>
+      </c>
+      <c r="O131" t="str">
+        <f t="shared" si="11"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="132" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A132" s="1">
+        <v>43109</v>
+      </c>
+      <c r="B132" s="2">
+        <v>3673</v>
+      </c>
+      <c r="C132" s="2">
+        <v>13366</v>
+      </c>
+      <c r="D132" s="3">
+        <v>10.41</v>
+      </c>
+      <c r="E132" s="2">
+        <v>4</v>
+      </c>
+      <c r="F132">
+        <v>559</v>
+      </c>
+      <c r="G132">
+        <v>382</v>
+      </c>
+      <c r="H132" s="2">
+        <v>3</v>
+      </c>
+      <c r="I132" s="2">
+        <v>24</v>
+      </c>
+      <c r="J132" s="2">
+        <v>2109</v>
+      </c>
+      <c r="K132" t="str">
+        <f t="shared" si="12"/>
+        <v>Yes</v>
+      </c>
+      <c r="L132" t="str">
+        <f t="shared" si="13"/>
+        <v>Yes</v>
+      </c>
+      <c r="M132" t="str">
+        <f t="shared" si="14"/>
+        <v>No</v>
+      </c>
+      <c r="N132" t="str">
+        <f t="shared" si="15"/>
+        <v>Yes</v>
+      </c>
+      <c r="O132" t="str">
+        <f t="shared" si="11"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="133" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A133" s="1">
+        <v>43110</v>
+      </c>
+      <c r="B133" s="2">
+        <v>4220</v>
+      </c>
+      <c r="C133" s="2">
+        <v>10799</v>
+      </c>
+      <c r="D133" s="3">
+        <v>7.99</v>
+      </c>
+      <c r="E133" s="2">
+        <v>9</v>
+      </c>
+      <c r="F133">
+        <v>568</v>
+      </c>
+      <c r="G133">
+        <v>337</v>
+      </c>
+      <c r="H133" s="2">
+        <v>29</v>
+      </c>
+      <c r="I133" s="2">
+        <v>65</v>
+      </c>
+      <c r="J133" s="2">
+        <v>2606</v>
+      </c>
+      <c r="K133" t="str">
+        <f t="shared" si="12"/>
+        <v>Yes</v>
+      </c>
+      <c r="L133" t="str">
+        <f t="shared" si="13"/>
+        <v>Yes</v>
+      </c>
+      <c r="M133" t="str">
+        <f t="shared" si="14"/>
+        <v>Yes</v>
+      </c>
+      <c r="N133" t="str">
+        <f t="shared" si="15"/>
+        <v>No</v>
+      </c>
+      <c r="O133" t="str">
+        <f t="shared" si="11"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="134" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A134" s="1">
+        <v>43111</v>
+      </c>
+      <c r="B134" s="2">
+        <v>4117</v>
+      </c>
+      <c r="C134" s="2">
+        <v>11812</v>
+      </c>
+      <c r="D134" s="3">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="E134" s="2">
+        <v>7</v>
+      </c>
+      <c r="F134">
+        <v>605</v>
+      </c>
+      <c r="G134">
+        <v>286</v>
+      </c>
+      <c r="H134" s="2">
+        <v>37</v>
+      </c>
+      <c r="I134" s="2">
+        <v>83</v>
+      </c>
+      <c r="J134" s="2">
+        <v>2528</v>
+      </c>
+      <c r="K134" t="str">
+        <f t="shared" si="12"/>
+        <v>Yes</v>
+      </c>
+      <c r="L134" t="str">
+        <f t="shared" si="13"/>
+        <v>Yes</v>
+      </c>
+      <c r="M134" t="str">
+        <f t="shared" si="14"/>
+        <v>Yes</v>
+      </c>
+      <c r="N134" t="str">
+        <f t="shared" si="15"/>
+        <v>No</v>
+      </c>
+      <c r="O134" t="str">
+        <f t="shared" si="11"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="135" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A135" s="1">
+        <v>43112</v>
+      </c>
+      <c r="B135" s="2">
+        <v>3692</v>
+      </c>
+      <c r="C135" s="2">
+        <v>13322</v>
+      </c>
+      <c r="D135" s="3">
+        <v>10.33</v>
+      </c>
+      <c r="E135" s="2">
+        <v>10</v>
+      </c>
+      <c r="F135">
+        <v>674</v>
+      </c>
+      <c r="G135">
+        <v>325</v>
+      </c>
+      <c r="H135" s="2">
+        <v>1</v>
+      </c>
+      <c r="I135" s="2">
+        <v>48</v>
+      </c>
+      <c r="J135" s="2">
+        <v>2084</v>
+      </c>
+      <c r="K135" t="str">
+        <f t="shared" si="12"/>
+        <v>Yes</v>
+      </c>
+      <c r="L135" t="str">
+        <f t="shared" si="13"/>
+        <v>Yes</v>
+      </c>
+      <c r="M135" t="str">
+        <f t="shared" si="14"/>
+        <v>Yes</v>
+      </c>
+      <c r="N135" t="str">
+        <f t="shared" si="15"/>
+        <v>No</v>
+      </c>
+      <c r="O135" t="str">
+        <f t="shared" si="11"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="136" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A136" s="1">
+        <v>43113</v>
+      </c>
+      <c r="B136" s="2">
+        <v>4149</v>
+      </c>
+      <c r="C136" s="2">
+        <v>9426</v>
+      </c>
+      <c r="D136" s="3">
+        <v>6.94</v>
+      </c>
+      <c r="E136" s="2">
+        <v>8</v>
+      </c>
+      <c r="F136">
+        <v>546</v>
+      </c>
+      <c r="G136">
+        <v>269</v>
+      </c>
+      <c r="H136" s="2">
+        <v>13</v>
+      </c>
+      <c r="I136" s="2">
+        <v>96</v>
+      </c>
+      <c r="J136" s="2">
+        <v>2513</v>
+      </c>
+      <c r="K136" t="str">
+        <f t="shared" si="12"/>
+        <v>Yes</v>
+      </c>
+      <c r="L136" t="str">
+        <f t="shared" si="13"/>
+        <v>Yes</v>
+      </c>
+      <c r="M136" t="str">
+        <f t="shared" si="14"/>
+        <v>Yes</v>
+      </c>
+      <c r="N136" t="str">
+        <f t="shared" si="15"/>
+        <v>No</v>
+      </c>
+      <c r="O136" t="str">
+        <f t="shared" si="11"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="137" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A137" s="1">
+        <v>43114</v>
+      </c>
+      <c r="B137" s="2">
+        <v>3862</v>
+      </c>
+      <c r="C137" s="2">
+        <v>11402</v>
+      </c>
+      <c r="D137" s="3">
+        <v>8.5500000000000007</v>
+      </c>
+      <c r="E137" s="2">
+        <v>14</v>
+      </c>
+      <c r="F137">
+        <v>611</v>
+      </c>
+      <c r="G137">
+        <v>298</v>
+      </c>
+      <c r="H137" s="2">
+        <v>29</v>
+      </c>
+      <c r="I137" s="2">
+        <v>55</v>
+      </c>
+      <c r="J137" s="2">
+        <v>2249</v>
+      </c>
+      <c r="K137" t="str">
+        <f t="shared" si="12"/>
+        <v>Yes</v>
+      </c>
+      <c r="L137" t="str">
+        <f t="shared" si="13"/>
+        <v>Yes</v>
+      </c>
+      <c r="M137" t="str">
+        <f t="shared" si="14"/>
+        <v>Yes</v>
+      </c>
+      <c r="N137" t="str">
+        <f t="shared" si="15"/>
+        <v>No</v>
+      </c>
+      <c r="O137" t="str">
+        <f t="shared" si="11"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="138" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A138" s="1">
+        <v>43115</v>
+      </c>
+      <c r="B138" s="2">
+        <v>4394</v>
+      </c>
+      <c r="C138" s="2">
+        <v>15077</v>
+      </c>
+      <c r="D138" s="3">
+        <v>11.42</v>
+      </c>
+      <c r="E138" s="2">
+        <v>25</v>
+      </c>
+      <c r="F138">
+        <v>456</v>
+      </c>
+      <c r="G138">
+        <v>421</v>
+      </c>
+      <c r="H138" s="2">
+        <v>28</v>
+      </c>
+      <c r="I138" s="2">
+        <v>66</v>
+      </c>
+      <c r="J138" s="2">
+        <v>2959</v>
+      </c>
+      <c r="K138" t="str">
+        <f t="shared" si="12"/>
+        <v>Yes</v>
+      </c>
+      <c r="L138" t="str">
+        <f t="shared" si="13"/>
+        <v>Yes</v>
+      </c>
+      <c r="M138" t="str">
+        <f t="shared" si="14"/>
+        <v>Yes</v>
+      </c>
+      <c r="N138" t="str">
+        <f t="shared" si="15"/>
+        <v>No</v>
+      </c>
+      <c r="O138" t="str">
+        <f t="shared" si="11"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="139" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A139" s="1">
+        <v>43116</v>
+      </c>
+      <c r="B139" s="2">
+        <v>3853</v>
+      </c>
+      <c r="C139" s="2">
+        <v>14420</v>
+      </c>
+      <c r="D139" s="3">
+        <v>11.24</v>
+      </c>
+      <c r="E139" s="2">
+        <v>20</v>
+      </c>
+      <c r="F139">
+        <v>531</v>
+      </c>
+      <c r="G139">
+        <v>360</v>
+      </c>
+      <c r="H139" s="2">
+        <v>1</v>
+      </c>
+      <c r="I139" s="2">
+        <v>51</v>
+      </c>
+      <c r="J139" s="2">
+        <v>2299</v>
+      </c>
+      <c r="K139" t="str">
+        <f t="shared" si="12"/>
+        <v>Yes</v>
+      </c>
+      <c r="L139" t="str">
+        <f t="shared" si="13"/>
+        <v>Yes</v>
+      </c>
+      <c r="M139" t="str">
+        <f t="shared" si="14"/>
+        <v>Yes</v>
+      </c>
+      <c r="N139" t="str">
+        <f t="shared" si="15"/>
+        <v>No</v>
+      </c>
+      <c r="O139" t="str">
+        <f t="shared" si="11"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="140" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A140" s="1">
+        <v>43117</v>
+      </c>
+      <c r="B140" s="2">
+        <v>4537</v>
+      </c>
+      <c r="C140" s="2">
+        <v>14452</v>
+      </c>
+      <c r="D140" s="3">
+        <v>10.77</v>
+      </c>
+      <c r="E140" s="2">
+        <v>20</v>
+      </c>
+      <c r="F140">
+        <v>512</v>
+      </c>
+      <c r="G140">
+        <v>349</v>
+      </c>
+      <c r="H140" s="2">
+        <v>25</v>
+      </c>
+      <c r="I140" s="2">
+        <v>102</v>
+      </c>
+      <c r="J140" s="2">
+        <v>3047</v>
+      </c>
+      <c r="K140" t="str">
+        <f t="shared" si="12"/>
+        <v>Yes</v>
+      </c>
+      <c r="L140" t="str">
+        <f t="shared" si="13"/>
+        <v>Yes</v>
+      </c>
+      <c r="M140" t="str">
+        <f t="shared" si="14"/>
+        <v>Yes</v>
+      </c>
+      <c r="N140" t="str">
+        <f t="shared" si="15"/>
+        <v>No</v>
+      </c>
+      <c r="O140" t="str">
+        <f t="shared" si="11"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="141" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A141" s="1">
+        <v>43118</v>
+      </c>
+      <c r="B141" s="2">
+        <v>4204</v>
+      </c>
+      <c r="C141" s="2">
+        <v>13200</v>
+      </c>
+      <c r="D141" s="3">
+        <v>9.89</v>
+      </c>
+      <c r="E141" s="2">
+        <v>12</v>
+      </c>
+      <c r="F141">
+        <v>332</v>
+      </c>
+      <c r="G141">
+        <v>396</v>
+      </c>
+      <c r="H141" s="2">
+        <v>29</v>
+      </c>
+      <c r="I141" s="2">
+        <v>68</v>
+      </c>
+      <c r="J141" s="2">
+        <v>2747</v>
+      </c>
+      <c r="K141" t="str">
+        <f t="shared" si="12"/>
+        <v>Yes</v>
+      </c>
+      <c r="L141" t="str">
+        <f t="shared" si="13"/>
+        <v>Yes</v>
+      </c>
+      <c r="M141" t="str">
+        <f t="shared" si="14"/>
+        <v>Yes</v>
+      </c>
+      <c r="N141" t="str">
+        <f t="shared" si="15"/>
+        <v>No</v>
+      </c>
+      <c r="O141" t="str">
+        <f t="shared" si="11"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="142" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A142" s="1">
+        <v>43119</v>
+      </c>
+      <c r="B142" s="2">
+        <v>4315</v>
+      </c>
+      <c r="C142" s="2">
+        <v>13618</v>
+      </c>
+      <c r="D142" s="3">
+        <v>10.16</v>
+      </c>
+      <c r="E142" s="2">
+        <v>10</v>
+      </c>
+      <c r="F142">
+        <v>660</v>
+      </c>
+      <c r="G142">
+        <v>394</v>
+      </c>
+      <c r="H142" s="2">
+        <v>29</v>
+      </c>
+      <c r="I142" s="2">
+        <v>73</v>
+      </c>
+      <c r="J142" s="2">
+        <v>2862</v>
+      </c>
+      <c r="K142" t="str">
+        <f t="shared" si="12"/>
+        <v>Yes</v>
+      </c>
+      <c r="L142" t="str">
+        <f t="shared" si="13"/>
+        <v>Yes</v>
+      </c>
+      <c r="M142" t="str">
+        <f t="shared" si="14"/>
+        <v>Yes</v>
+      </c>
+      <c r="N142" t="str">
+        <f t="shared" si="15"/>
+        <v>No</v>
+      </c>
+      <c r="O142" t="str">
+        <f t="shared" si="11"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="143" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A143" s="1">
+        <v>43120</v>
+      </c>
+      <c r="B143" s="2">
+        <v>3607</v>
+      </c>
+      <c r="C143" s="2">
+        <v>11996</v>
+      </c>
+      <c r="D143" s="3">
+        <v>9.3699999999999992</v>
+      </c>
+      <c r="E143" s="2">
+        <v>13</v>
+      </c>
+      <c r="F143">
+        <v>539</v>
+      </c>
+      <c r="G143">
+        <v>317</v>
+      </c>
+      <c r="H143" s="2">
+        <v>2</v>
+      </c>
+      <c r="I143" s="2">
+        <v>50</v>
+      </c>
+      <c r="J143" s="2">
+        <v>2003</v>
+      </c>
+      <c r="K143" t="str">
+        <f t="shared" si="12"/>
+        <v>Yes</v>
+      </c>
+      <c r="L143" t="str">
+        <f t="shared" si="13"/>
+        <v>Yes</v>
+      </c>
+      <c r="M143" t="str">
+        <f t="shared" si="14"/>
+        <v>Yes</v>
+      </c>
+      <c r="N143" t="str">
+        <f t="shared" si="15"/>
+        <v>No</v>
+      </c>
+      <c r="O143" t="str">
+        <f t="shared" si="11"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="144" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A144" s="1">
+        <v>43121</v>
+      </c>
+      <c r="B144" s="2">
+        <v>3701</v>
+      </c>
+      <c r="C144" s="2">
+        <v>10698</v>
+      </c>
+      <c r="D144" s="3">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="E144" s="2">
+        <v>10</v>
+      </c>
+      <c r="F144">
+        <v>577</v>
+      </c>
+      <c r="G144">
+        <v>320</v>
+      </c>
+      <c r="H144" s="2">
+        <v>25</v>
+      </c>
+      <c r="I144" s="2">
+        <v>45</v>
+      </c>
+      <c r="J144" s="2">
+        <v>2128</v>
+      </c>
+      <c r="K144" t="str">
+        <f t="shared" si="12"/>
+        <v>Yes</v>
+      </c>
+      <c r="L144" t="str">
+        <f t="shared" si="13"/>
+        <v>Yes</v>
+      </c>
+      <c r="M144" t="str">
+        <f t="shared" si="14"/>
+        <v>Yes</v>
+      </c>
+      <c r="N144" t="str">
+        <f t="shared" si="15"/>
+        <v>No</v>
+      </c>
+      <c r="O144" t="str">
+        <f t="shared" si="11"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="145" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A145" s="1">
+        <v>43122</v>
+      </c>
+      <c r="B145" s="2">
+        <v>4195</v>
+      </c>
+      <c r="C145" s="2">
+        <v>13754</v>
+      </c>
+      <c r="D145" s="3">
+        <v>10.31</v>
+      </c>
+      <c r="E145" s="2">
+        <v>10</v>
+      </c>
+      <c r="F145">
+        <v>468</v>
+      </c>
+      <c r="G145">
+        <v>419</v>
+      </c>
+      <c r="H145" s="2">
+        <v>43</v>
+      </c>
+      <c r="I145" s="2">
+        <v>51</v>
+      </c>
+      <c r="J145" s="2">
+        <v>2756</v>
+      </c>
+      <c r="K145" t="str">
+        <f t="shared" si="12"/>
+        <v>Yes</v>
+      </c>
+      <c r="L145" t="str">
+        <f t="shared" si="13"/>
+        <v>Yes</v>
+      </c>
+      <c r="M145" t="str">
+        <f t="shared" si="14"/>
+        <v>Yes</v>
+      </c>
+      <c r="N145" t="str">
+        <f t="shared" si="15"/>
+        <v>No</v>
+      </c>
+      <c r="O145" t="str">
+        <f t="shared" si="11"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="146" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A146" s="1">
+        <v>43123</v>
+      </c>
+      <c r="B146" s="2">
+        <v>3152</v>
+      </c>
+      <c r="C146" s="2">
+        <v>8121</v>
+      </c>
+      <c r="D146" s="3">
+        <v>6.33</v>
+      </c>
+      <c r="E146" s="2">
+        <v>4</v>
+      </c>
+      <c r="F146">
+        <v>640</v>
+      </c>
+      <c r="G146">
+        <v>336</v>
+      </c>
+      <c r="H146" s="2">
+        <v>0</v>
+      </c>
+      <c r="I146" s="2">
+        <v>0</v>
+      </c>
+      <c r="J146" s="2">
+        <v>1504</v>
+      </c>
+      <c r="K146" t="str">
+        <f t="shared" si="12"/>
+        <v>Yes</v>
+      </c>
+      <c r="L146" t="str">
+        <f t="shared" si="13"/>
+        <v>No</v>
+      </c>
+      <c r="M146" t="str">
+        <f t="shared" si="14"/>
+        <v>No</v>
+      </c>
+      <c r="N146" t="str">
+        <f t="shared" si="15"/>
+        <v>Yes</v>
+      </c>
+      <c r="O146" t="str">
+        <f t="shared" si="11"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="147" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A147" s="1">
+        <v>43124</v>
+      </c>
+      <c r="B147" s="2">
+        <v>2531</v>
+      </c>
+      <c r="C147" s="2">
+        <v>1331</v>
+      </c>
+      <c r="D147" s="3">
+        <v>1.04</v>
+      </c>
+      <c r="E147" s="2">
+        <v>7</v>
+      </c>
+      <c r="F147">
+        <v>735</v>
+      </c>
+      <c r="G147">
+        <v>87</v>
+      </c>
+      <c r="H147" s="2">
+        <v>0</v>
+      </c>
+      <c r="I147" s="2">
+        <v>0</v>
+      </c>
+      <c r="J147" s="2">
+        <v>379</v>
+      </c>
+      <c r="K147" t="str">
+        <f t="shared" si="12"/>
+        <v>No</v>
+      </c>
+      <c r="L147" t="str">
+        <f t="shared" si="13"/>
+        <v>No</v>
+      </c>
+      <c r="M147" t="str">
+        <f t="shared" si="14"/>
+        <v>No</v>
+      </c>
+      <c r="N147" t="str">
+        <f t="shared" si="15"/>
+        <v>Yes</v>
+      </c>
+      <c r="O147" t="str">
+        <f t="shared" si="11"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="148" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A148" s="1">
+        <v>43125</v>
+      </c>
+      <c r="B148" s="2">
+        <v>2859</v>
+      </c>
+      <c r="C148" s="2">
+        <v>5871</v>
+      </c>
+      <c r="D148" s="3">
+        <v>4.58</v>
+      </c>
+      <c r="E148" s="2">
+        <v>1</v>
+      </c>
+      <c r="F148">
+        <v>614</v>
+      </c>
+      <c r="G148">
+        <v>233</v>
+      </c>
+      <c r="H148" s="2">
+        <v>0</v>
+      </c>
+      <c r="I148" s="2">
+        <v>0</v>
+      </c>
+      <c r="J148" s="2">
+        <v>1075</v>
+      </c>
+      <c r="K148" t="str">
+        <f t="shared" si="12"/>
+        <v>No</v>
+      </c>
+      <c r="L148" t="str">
+        <f t="shared" si="13"/>
+        <v>No</v>
+      </c>
+      <c r="M148" t="str">
+        <f t="shared" si="14"/>
+        <v>No</v>
+      </c>
+      <c r="N148" t="str">
+        <f t="shared" si="15"/>
+        <v>Yes</v>
+      </c>
+      <c r="O148" t="str">
+        <f t="shared" si="11"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="149" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A149" s="1">
+        <v>43126</v>
+      </c>
+      <c r="B149" s="2">
+        <v>3434</v>
+      </c>
+      <c r="C149" s="2">
+        <v>11191</v>
+      </c>
+      <c r="D149" s="3">
+        <v>8.73</v>
+      </c>
+      <c r="E149" s="2">
+        <v>1</v>
+      </c>
+      <c r="F149">
+        <v>537</v>
+      </c>
+      <c r="G149">
+        <v>406</v>
+      </c>
+      <c r="H149" s="2">
+        <v>11</v>
+      </c>
+      <c r="I149" s="2">
+        <v>0</v>
+      </c>
+      <c r="J149" s="2">
+        <v>1917</v>
+      </c>
+      <c r="K149" t="str">
+        <f t="shared" si="12"/>
+        <v>Yes</v>
+      </c>
+      <c r="L149" t="str">
+        <f t="shared" si="13"/>
+        <v>Yes</v>
+      </c>
+      <c r="M149" t="str">
+        <f t="shared" si="14"/>
+        <v>No</v>
+      </c>
+      <c r="N149" t="str">
+        <f t="shared" si="15"/>
+        <v>Yes</v>
+      </c>
+      <c r="O149" t="str">
+        <f t="shared" si="11"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="150" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A150" s="1">
+        <v>43127</v>
+      </c>
+      <c r="B150" s="2">
+        <v>3442</v>
+      </c>
+      <c r="C150" s="2">
+        <v>10370</v>
+      </c>
+      <c r="D150" s="3">
+        <v>8.09</v>
+      </c>
+      <c r="E150" s="2">
+        <v>1</v>
+      </c>
+      <c r="F150">
+        <v>638</v>
+      </c>
+      <c r="G150">
+        <v>453</v>
+      </c>
+      <c r="H150" s="2">
+        <v>0</v>
+      </c>
+      <c r="I150" s="2">
+        <v>0</v>
+      </c>
+      <c r="J150" s="2">
+        <v>1952</v>
+      </c>
+      <c r="K150" t="str">
+        <f t="shared" si="12"/>
+        <v>Yes</v>
+      </c>
+      <c r="L150" t="str">
+        <f t="shared" si="13"/>
+        <v>Yes</v>
+      </c>
+      <c r="M150" t="str">
+        <f t="shared" si="14"/>
+        <v>No</v>
+      </c>
+      <c r="N150" t="str">
+        <f t="shared" si="15"/>
+        <v>Yes</v>
+      </c>
+      <c r="O150" t="str">
+        <f t="shared" si="11"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="151" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A151" s="1">
+        <v>43128</v>
+      </c>
+      <c r="B151" s="2">
+        <v>3036</v>
+      </c>
+      <c r="C151" s="2">
+        <v>7198</v>
+      </c>
+      <c r="D151" s="3">
+        <v>5.61</v>
+      </c>
+      <c r="E151" s="2">
+        <v>3</v>
+      </c>
+      <c r="F151">
+        <v>615</v>
+      </c>
+      <c r="G151">
+        <v>252</v>
+      </c>
+      <c r="H151" s="2">
+        <v>0</v>
+      </c>
+      <c r="I151" s="2">
+        <v>0</v>
+      </c>
+      <c r="J151" s="2">
+        <v>1208</v>
+      </c>
+      <c r="K151" t="str">
+        <f t="shared" si="12"/>
+        <v>No</v>
+      </c>
+      <c r="L151" t="str">
+        <f t="shared" si="13"/>
+        <v>No</v>
+      </c>
+      <c r="M151" t="str">
+        <f t="shared" si="14"/>
+        <v>No</v>
+      </c>
+      <c r="N151" t="str">
+        <f t="shared" si="15"/>
+        <v>Yes</v>
+      </c>
+      <c r="O151" t="str">
+        <f t="shared" si="11"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="152" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A152" s="1">
+        <v>43129</v>
+      </c>
+      <c r="B152" s="2">
+        <v>2544</v>
+      </c>
+      <c r="C152" s="2">
+        <v>3834</v>
+      </c>
+      <c r="D152" s="3">
+        <v>2.99</v>
+      </c>
+      <c r="E152" s="2">
+        <v>4</v>
+      </c>
+      <c r="F152" s="4">
+        <v>1345</v>
+      </c>
+      <c r="G152">
+        <v>86</v>
+      </c>
+      <c r="H152" s="2">
+        <v>5</v>
+      </c>
+      <c r="I152" s="2">
+        <v>4</v>
+      </c>
+      <c r="J152" s="2">
+        <v>536</v>
+      </c>
+      <c r="K152" t="str">
+        <f t="shared" si="12"/>
+        <v>No</v>
+      </c>
+      <c r="L152" t="str">
+        <f t="shared" si="13"/>
+        <v>No</v>
+      </c>
+      <c r="M152" t="str">
+        <f t="shared" si="14"/>
+        <v>No</v>
+      </c>
+      <c r="N152" t="str">
+        <f t="shared" si="15"/>
+        <v>Yes</v>
+      </c>
+      <c r="O152" t="str">
+        <f t="shared" si="11"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="153" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A153" s="1">
+        <v>43130</v>
+      </c>
+      <c r="B153" s="2">
+        <v>3396</v>
+      </c>
+      <c r="C153" s="2">
+        <v>10480</v>
+      </c>
+      <c r="D153" s="3">
+        <v>8.17</v>
+      </c>
+      <c r="E153" s="2">
+        <v>17</v>
+      </c>
+      <c r="F153" s="4">
+        <v>1070</v>
+      </c>
+      <c r="G153">
+        <v>243</v>
+      </c>
+      <c r="H153" s="2">
+        <v>17</v>
+      </c>
+      <c r="I153" s="2">
+        <v>40</v>
+      </c>
+      <c r="J153" s="2">
+        <v>1685</v>
+      </c>
+      <c r="K153" t="str">
+        <f t="shared" si="12"/>
+        <v>Yes</v>
+      </c>
+      <c r="L153" t="str">
+        <f t="shared" si="13"/>
+        <v>No</v>
+      </c>
+      <c r="M153" t="str">
+        <f t="shared" si="14"/>
+        <v>Yes</v>
+      </c>
+      <c r="N153" t="str">
+        <f t="shared" si="15"/>
+        <v>No</v>
+      </c>
+      <c r="O153" t="str">
+        <f t="shared" si="11"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="154" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A154" s="1">
+        <v>43131</v>
+      </c>
+      <c r="B154" s="2">
+        <v>4390</v>
+      </c>
+      <c r="C154" s="2">
+        <v>12902</v>
+      </c>
+      <c r="D154" s="3">
+        <v>9.92</v>
+      </c>
+      <c r="E154" s="2">
+        <v>20</v>
+      </c>
+      <c r="F154">
+        <v>506</v>
+      </c>
+      <c r="G154">
+        <v>291</v>
+      </c>
+      <c r="H154" s="2">
+        <v>68</v>
+      </c>
+      <c r="I154" s="2">
+        <v>92</v>
+      </c>
+      <c r="J154" s="2">
+        <v>2862</v>
+      </c>
+      <c r="K154" t="str">
+        <f t="shared" si="12"/>
+        <v>Yes</v>
+      </c>
+      <c r="L154" t="str">
+        <f t="shared" si="13"/>
+        <v>Yes</v>
+      </c>
+      <c r="M154" t="str">
+        <f t="shared" si="14"/>
+        <v>Yes</v>
+      </c>
+      <c r="N154" t="str">
+        <f t="shared" si="15"/>
+        <v>No</v>
+      </c>
+      <c r="O154" t="str">
+        <f t="shared" si="11"/>
         <v>Yes</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updating TotalExercise file for February numbers
</commit_message>
<xml_diff>
--- a/datasets/TotalExercise.xlsx
+++ b/datasets/TotalExercise.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -208,6 +208,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -914,10 +915,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O154"/>
+  <dimension ref="A1:O182"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O123" sqref="O123:O154"/>
+      <selection activeCell="O154" sqref="O154:O182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6647,7 +6648,7 @@
         <v>Yes</v>
       </c>
       <c r="O110" t="str">
-        <f t="shared" ref="O110:O154" si="11">IF(D110&gt;5,"Yes","No")</f>
+        <f t="shared" ref="O110:O173" si="11">IF(D110&gt;5,"Yes","No")</f>
         <v>No</v>
       </c>
     </row>
@@ -7723,19 +7724,19 @@
         <v>2017</v>
       </c>
       <c r="K131" t="str">
-        <f t="shared" ref="K131:K154" si="12">IF(C131&gt;8000,"Yes","No")</f>
+        <f t="shared" ref="K131:K182" si="12">IF(C131&gt;8000,"Yes","No")</f>
         <v>Yes</v>
       </c>
       <c r="L131" t="str">
-        <f t="shared" ref="L131:L154" si="13">IF(B131&gt;3400,"Yes","No")</f>
+        <f t="shared" ref="L131:L182" si="13">IF(B131&gt;3400,"Yes","No")</f>
         <v>Yes</v>
       </c>
       <c r="M131" t="str">
-        <f t="shared" ref="M131:M154" si="14">IF(I131&gt;30,"Yes","No")</f>
+        <f t="shared" ref="M131:M182" si="14">IF(I131&gt;30,"Yes","No")</f>
         <v>Yes</v>
       </c>
       <c r="N131" t="str">
-        <f t="shared" ref="N131:N154" si="15">IF(I131+H131&lt;30,"Yes","No")</f>
+        <f t="shared" ref="N131:N182" si="15">IF(I131+H131&lt;30,"Yes","No")</f>
         <v>No</v>
       </c>
       <c r="O131" t="str">
@@ -8936,6 +8937,1462 @@
       </c>
       <c r="O154" t="str">
         <f t="shared" si="11"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="155" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A155" s="1">
+        <v>43132</v>
+      </c>
+      <c r="B155" s="2">
+        <v>3133</v>
+      </c>
+      <c r="C155" s="2">
+        <v>7442</v>
+      </c>
+      <c r="D155" s="2">
+        <v>5.8</v>
+      </c>
+      <c r="E155" s="2">
+        <v>6</v>
+      </c>
+      <c r="F155" s="2">
+        <v>911</v>
+      </c>
+      <c r="G155" s="2">
+        <v>281</v>
+      </c>
+      <c r="H155" s="2">
+        <v>7</v>
+      </c>
+      <c r="I155" s="2">
+        <v>0</v>
+      </c>
+      <c r="J155" s="2">
+        <v>1376</v>
+      </c>
+      <c r="K155" t="str">
+        <f t="shared" si="12"/>
+        <v>No</v>
+      </c>
+      <c r="L155" t="str">
+        <f t="shared" si="13"/>
+        <v>No</v>
+      </c>
+      <c r="M155" t="str">
+        <f t="shared" si="14"/>
+        <v>No</v>
+      </c>
+      <c r="N155" t="str">
+        <f t="shared" si="15"/>
+        <v>Yes</v>
+      </c>
+      <c r="O155" t="str">
+        <f t="shared" si="11"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="156" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A156" s="1">
+        <v>43133</v>
+      </c>
+      <c r="B156" s="2">
+        <v>3535</v>
+      </c>
+      <c r="C156" s="2">
+        <v>8304</v>
+      </c>
+      <c r="D156" s="2">
+        <v>6.3</v>
+      </c>
+      <c r="E156" s="2">
+        <v>10</v>
+      </c>
+      <c r="F156" s="2">
+        <v>698</v>
+      </c>
+      <c r="G156" s="2">
+        <v>298</v>
+      </c>
+      <c r="H156" s="2">
+        <v>22</v>
+      </c>
+      <c r="I156" s="2">
+        <v>13</v>
+      </c>
+      <c r="J156" s="2">
+        <v>1778</v>
+      </c>
+      <c r="K156" t="str">
+        <f t="shared" si="12"/>
+        <v>Yes</v>
+      </c>
+      <c r="L156" t="str">
+        <f t="shared" si="13"/>
+        <v>Yes</v>
+      </c>
+      <c r="M156" t="str">
+        <f t="shared" si="14"/>
+        <v>No</v>
+      </c>
+      <c r="N156" t="str">
+        <f t="shared" si="15"/>
+        <v>No</v>
+      </c>
+      <c r="O156" t="str">
+        <f t="shared" si="11"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="157" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A157" s="1">
+        <v>43134</v>
+      </c>
+      <c r="B157" s="2">
+        <v>3322</v>
+      </c>
+      <c r="C157" s="2">
+        <v>10198</v>
+      </c>
+      <c r="D157" s="2">
+        <v>7.95</v>
+      </c>
+      <c r="E157" s="2">
+        <v>1</v>
+      </c>
+      <c r="F157" s="2">
+        <v>678</v>
+      </c>
+      <c r="G157" s="2">
+        <v>331</v>
+      </c>
+      <c r="H157" s="2">
+        <v>13</v>
+      </c>
+      <c r="I157" s="2">
+        <v>13</v>
+      </c>
+      <c r="J157" s="2">
+        <v>1684</v>
+      </c>
+      <c r="K157" t="str">
+        <f t="shared" si="12"/>
+        <v>Yes</v>
+      </c>
+      <c r="L157" t="str">
+        <f t="shared" si="13"/>
+        <v>No</v>
+      </c>
+      <c r="M157" t="str">
+        <f t="shared" si="14"/>
+        <v>No</v>
+      </c>
+      <c r="N157" t="str">
+        <f t="shared" si="15"/>
+        <v>Yes</v>
+      </c>
+      <c r="O157" t="str">
+        <f t="shared" si="11"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="158" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A158" s="1">
+        <v>43135</v>
+      </c>
+      <c r="B158" s="2">
+        <v>3030</v>
+      </c>
+      <c r="C158" s="2">
+        <v>6184</v>
+      </c>
+      <c r="D158" s="2">
+        <v>4.82</v>
+      </c>
+      <c r="E158" s="2">
+        <v>3</v>
+      </c>
+      <c r="F158" s="2">
+        <v>832</v>
+      </c>
+      <c r="G158" s="2">
+        <v>275</v>
+      </c>
+      <c r="H158" s="2">
+        <v>0</v>
+      </c>
+      <c r="I158" s="2">
+        <v>0</v>
+      </c>
+      <c r="J158" s="2">
+        <v>1241</v>
+      </c>
+      <c r="K158" t="str">
+        <f t="shared" si="12"/>
+        <v>No</v>
+      </c>
+      <c r="L158" t="str">
+        <f t="shared" si="13"/>
+        <v>No</v>
+      </c>
+      <c r="M158" t="str">
+        <f t="shared" si="14"/>
+        <v>No</v>
+      </c>
+      <c r="N158" t="str">
+        <f t="shared" si="15"/>
+        <v>Yes</v>
+      </c>
+      <c r="O158" t="str">
+        <f t="shared" si="11"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="159" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A159" s="1">
+        <v>43136</v>
+      </c>
+      <c r="B159" s="2">
+        <v>4186</v>
+      </c>
+      <c r="C159" s="2">
+        <v>9442</v>
+      </c>
+      <c r="D159" s="2">
+        <v>7.07</v>
+      </c>
+      <c r="E159" s="2">
+        <v>13</v>
+      </c>
+      <c r="F159" s="2">
+        <v>697</v>
+      </c>
+      <c r="G159" s="2">
+        <v>289</v>
+      </c>
+      <c r="H159" s="2">
+        <v>8</v>
+      </c>
+      <c r="I159" s="2">
+        <v>100</v>
+      </c>
+      <c r="J159" s="2">
+        <v>2573</v>
+      </c>
+      <c r="K159" t="str">
+        <f t="shared" si="12"/>
+        <v>Yes</v>
+      </c>
+      <c r="L159" t="str">
+        <f t="shared" si="13"/>
+        <v>Yes</v>
+      </c>
+      <c r="M159" t="str">
+        <f t="shared" si="14"/>
+        <v>Yes</v>
+      </c>
+      <c r="N159" t="str">
+        <f t="shared" si="15"/>
+        <v>No</v>
+      </c>
+      <c r="O159" t="str">
+        <f t="shared" si="11"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="160" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A160" s="1">
+        <v>43137</v>
+      </c>
+      <c r="B160" s="2">
+        <v>4257</v>
+      </c>
+      <c r="C160" s="2">
+        <v>10638</v>
+      </c>
+      <c r="D160" s="2">
+        <v>7.95</v>
+      </c>
+      <c r="E160" s="2">
+        <v>14</v>
+      </c>
+      <c r="F160" s="2">
+        <v>563</v>
+      </c>
+      <c r="G160" s="2">
+        <v>283</v>
+      </c>
+      <c r="H160" s="2">
+        <v>62</v>
+      </c>
+      <c r="I160" s="2">
+        <v>69</v>
+      </c>
+      <c r="J160" s="2">
+        <v>2661</v>
+      </c>
+      <c r="K160" t="str">
+        <f t="shared" si="12"/>
+        <v>Yes</v>
+      </c>
+      <c r="L160" t="str">
+        <f t="shared" si="13"/>
+        <v>Yes</v>
+      </c>
+      <c r="M160" t="str">
+        <f t="shared" si="14"/>
+        <v>Yes</v>
+      </c>
+      <c r="N160" t="str">
+        <f t="shared" si="15"/>
+        <v>No</v>
+      </c>
+      <c r="O160" t="str">
+        <f t="shared" si="11"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="161" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A161" s="1">
+        <v>43138</v>
+      </c>
+      <c r="B161" s="2">
+        <v>3455</v>
+      </c>
+      <c r="C161" s="2">
+        <v>12744</v>
+      </c>
+      <c r="D161" s="2">
+        <v>9.94</v>
+      </c>
+      <c r="E161" s="2">
+        <v>17</v>
+      </c>
+      <c r="F161" s="2">
+        <v>734</v>
+      </c>
+      <c r="G161" s="2">
+        <v>249</v>
+      </c>
+      <c r="H161" s="2">
+        <v>18</v>
+      </c>
+      <c r="I161" s="2">
+        <v>44</v>
+      </c>
+      <c r="J161" s="2">
+        <v>1768</v>
+      </c>
+      <c r="K161" t="str">
+        <f t="shared" si="12"/>
+        <v>Yes</v>
+      </c>
+      <c r="L161" t="str">
+        <f t="shared" si="13"/>
+        <v>Yes</v>
+      </c>
+      <c r="M161" t="str">
+        <f t="shared" si="14"/>
+        <v>Yes</v>
+      </c>
+      <c r="N161" t="str">
+        <f t="shared" si="15"/>
+        <v>No</v>
+      </c>
+      <c r="O161" t="str">
+        <f t="shared" si="11"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="162" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A162" s="1">
+        <v>43139</v>
+      </c>
+      <c r="B162" s="2">
+        <v>4186</v>
+      </c>
+      <c r="C162" s="2">
+        <v>11519</v>
+      </c>
+      <c r="D162" s="2">
+        <v>8.69</v>
+      </c>
+      <c r="E162" s="2">
+        <v>16</v>
+      </c>
+      <c r="F162" s="2">
+        <v>693</v>
+      </c>
+      <c r="G162" s="2">
+        <v>306</v>
+      </c>
+      <c r="H162" s="2">
+        <v>29</v>
+      </c>
+      <c r="I162" s="2">
+        <v>75</v>
+      </c>
+      <c r="J162" s="2">
+        <v>2584</v>
+      </c>
+      <c r="K162" t="str">
+        <f t="shared" si="12"/>
+        <v>Yes</v>
+      </c>
+      <c r="L162" t="str">
+        <f t="shared" si="13"/>
+        <v>Yes</v>
+      </c>
+      <c r="M162" t="str">
+        <f t="shared" si="14"/>
+        <v>Yes</v>
+      </c>
+      <c r="N162" t="str">
+        <f t="shared" si="15"/>
+        <v>No</v>
+      </c>
+      <c r="O162" t="str">
+        <f t="shared" si="11"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="163" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A163" s="1">
+        <v>43140</v>
+      </c>
+      <c r="B163" s="2">
+        <v>4036</v>
+      </c>
+      <c r="C163" s="2">
+        <v>10010</v>
+      </c>
+      <c r="D163" s="2">
+        <v>7.5</v>
+      </c>
+      <c r="E163" s="2">
+        <v>10</v>
+      </c>
+      <c r="F163" s="2">
+        <v>579</v>
+      </c>
+      <c r="G163" s="2">
+        <v>315</v>
+      </c>
+      <c r="H163" s="2">
+        <v>36</v>
+      </c>
+      <c r="I163" s="2">
+        <v>61</v>
+      </c>
+      <c r="J163" s="2">
+        <v>2459</v>
+      </c>
+      <c r="K163" t="str">
+        <f t="shared" si="12"/>
+        <v>Yes</v>
+      </c>
+      <c r="L163" t="str">
+        <f t="shared" si="13"/>
+        <v>Yes</v>
+      </c>
+      <c r="M163" t="str">
+        <f t="shared" si="14"/>
+        <v>Yes</v>
+      </c>
+      <c r="N163" t="str">
+        <f t="shared" si="15"/>
+        <v>No</v>
+      </c>
+      <c r="O163" t="str">
+        <f t="shared" si="11"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="164" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A164" s="1">
+        <v>43141</v>
+      </c>
+      <c r="B164" s="2">
+        <v>3291</v>
+      </c>
+      <c r="C164" s="2">
+        <v>9633</v>
+      </c>
+      <c r="D164" s="2">
+        <v>7.51</v>
+      </c>
+      <c r="E164" s="2">
+        <v>17</v>
+      </c>
+      <c r="F164" s="2">
+        <v>620</v>
+      </c>
+      <c r="G164" s="2">
+        <v>340</v>
+      </c>
+      <c r="H164" s="2">
+        <v>0</v>
+      </c>
+      <c r="I164" s="2">
+        <v>0</v>
+      </c>
+      <c r="J164" s="2">
+        <v>1631</v>
+      </c>
+      <c r="K164" t="str">
+        <f t="shared" si="12"/>
+        <v>Yes</v>
+      </c>
+      <c r="L164" t="str">
+        <f t="shared" si="13"/>
+        <v>No</v>
+      </c>
+      <c r="M164" t="str">
+        <f t="shared" si="14"/>
+        <v>No</v>
+      </c>
+      <c r="N164" t="str">
+        <f t="shared" si="15"/>
+        <v>Yes</v>
+      </c>
+      <c r="O164" t="str">
+        <f t="shared" si="11"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="165" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A165" s="1">
+        <v>43142</v>
+      </c>
+      <c r="B165" s="2">
+        <v>4034</v>
+      </c>
+      <c r="C165" s="2">
+        <v>10468</v>
+      </c>
+      <c r="D165" s="2">
+        <v>7.88</v>
+      </c>
+      <c r="E165" s="2">
+        <v>7</v>
+      </c>
+      <c r="F165" s="2">
+        <v>513</v>
+      </c>
+      <c r="G165" s="2">
+        <v>324</v>
+      </c>
+      <c r="H165" s="2">
+        <v>69</v>
+      </c>
+      <c r="I165" s="2">
+        <v>52</v>
+      </c>
+      <c r="J165" s="2">
+        <v>2522</v>
+      </c>
+      <c r="K165" t="str">
+        <f t="shared" si="12"/>
+        <v>Yes</v>
+      </c>
+      <c r="L165" t="str">
+        <f t="shared" si="13"/>
+        <v>Yes</v>
+      </c>
+      <c r="M165" t="str">
+        <f t="shared" si="14"/>
+        <v>Yes</v>
+      </c>
+      <c r="N165" t="str">
+        <f t="shared" si="15"/>
+        <v>No</v>
+      </c>
+      <c r="O165" t="str">
+        <f t="shared" si="11"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="166" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A166" s="1">
+        <v>43143</v>
+      </c>
+      <c r="B166" s="2">
+        <v>3754</v>
+      </c>
+      <c r="C166" s="2">
+        <v>9452</v>
+      </c>
+      <c r="D166" s="2">
+        <v>7.37</v>
+      </c>
+      <c r="E166" s="2">
+        <v>12</v>
+      </c>
+      <c r="F166" s="2">
+        <v>531</v>
+      </c>
+      <c r="G166" s="2">
+        <v>328</v>
+      </c>
+      <c r="H166" s="2">
+        <v>15</v>
+      </c>
+      <c r="I166" s="2">
+        <v>29</v>
+      </c>
+      <c r="J166" s="2">
+        <v>2013</v>
+      </c>
+      <c r="K166" t="str">
+        <f t="shared" si="12"/>
+        <v>Yes</v>
+      </c>
+      <c r="L166" t="str">
+        <f t="shared" si="13"/>
+        <v>Yes</v>
+      </c>
+      <c r="M166" t="str">
+        <f t="shared" si="14"/>
+        <v>No</v>
+      </c>
+      <c r="N166" t="str">
+        <f t="shared" si="15"/>
+        <v>No</v>
+      </c>
+      <c r="O166" t="str">
+        <f t="shared" si="11"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="167" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A167" s="1">
+        <v>43144</v>
+      </c>
+      <c r="B167" s="2">
+        <v>4613</v>
+      </c>
+      <c r="C167" s="2">
+        <v>14111</v>
+      </c>
+      <c r="D167" s="2">
+        <v>11.01</v>
+      </c>
+      <c r="E167" s="2">
+        <v>18</v>
+      </c>
+      <c r="F167" s="2">
+        <v>637</v>
+      </c>
+      <c r="G167" s="2">
+        <v>322</v>
+      </c>
+      <c r="H167" s="2">
+        <v>99</v>
+      </c>
+      <c r="I167" s="2">
+        <v>84</v>
+      </c>
+      <c r="J167" s="2">
+        <v>3109</v>
+      </c>
+      <c r="K167" t="str">
+        <f t="shared" si="12"/>
+        <v>Yes</v>
+      </c>
+      <c r="L167" t="str">
+        <f t="shared" si="13"/>
+        <v>Yes</v>
+      </c>
+      <c r="M167" t="str">
+        <f t="shared" si="14"/>
+        <v>Yes</v>
+      </c>
+      <c r="N167" t="str">
+        <f t="shared" si="15"/>
+        <v>No</v>
+      </c>
+      <c r="O167" t="str">
+        <f t="shared" si="11"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="168" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A168" s="1">
+        <v>43145</v>
+      </c>
+      <c r="B168" s="2">
+        <v>3437</v>
+      </c>
+      <c r="C168" s="2">
+        <v>9294</v>
+      </c>
+      <c r="D168" s="2">
+        <v>7.25</v>
+      </c>
+      <c r="E168" s="2">
+        <v>9</v>
+      </c>
+      <c r="F168" s="2">
+        <v>928</v>
+      </c>
+      <c r="G168" s="2">
+        <v>354</v>
+      </c>
+      <c r="H168" s="2">
+        <v>0</v>
+      </c>
+      <c r="I168" s="2">
+        <v>0</v>
+      </c>
+      <c r="J168" s="2">
+        <v>1703</v>
+      </c>
+      <c r="K168" t="str">
+        <f t="shared" si="12"/>
+        <v>Yes</v>
+      </c>
+      <c r="L168" t="str">
+        <f t="shared" si="13"/>
+        <v>Yes</v>
+      </c>
+      <c r="M168" t="str">
+        <f t="shared" si="14"/>
+        <v>No</v>
+      </c>
+      <c r="N168" t="str">
+        <f t="shared" si="15"/>
+        <v>Yes</v>
+      </c>
+      <c r="O168" t="str">
+        <f t="shared" si="11"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="169" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A169" s="1">
+        <v>43146</v>
+      </c>
+      <c r="B169" s="2">
+        <v>3742</v>
+      </c>
+      <c r="C169" s="2">
+        <v>10974</v>
+      </c>
+      <c r="D169" s="2">
+        <v>8.35</v>
+      </c>
+      <c r="E169" s="2">
+        <v>12</v>
+      </c>
+      <c r="F169" s="2">
+        <v>621</v>
+      </c>
+      <c r="G169" s="2">
+        <v>284</v>
+      </c>
+      <c r="H169" s="2">
+        <v>27</v>
+      </c>
+      <c r="I169" s="2">
+        <v>43</v>
+      </c>
+      <c r="J169" s="2">
+        <v>2053</v>
+      </c>
+      <c r="K169" t="str">
+        <f t="shared" si="12"/>
+        <v>Yes</v>
+      </c>
+      <c r="L169" t="str">
+        <f t="shared" si="13"/>
+        <v>Yes</v>
+      </c>
+      <c r="M169" t="str">
+        <f t="shared" si="14"/>
+        <v>Yes</v>
+      </c>
+      <c r="N169" t="str">
+        <f t="shared" si="15"/>
+        <v>No</v>
+      </c>
+      <c r="O169" t="str">
+        <f t="shared" si="11"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="170" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A170" s="1">
+        <v>43147</v>
+      </c>
+      <c r="B170" s="2">
+        <v>3682</v>
+      </c>
+      <c r="C170" s="2">
+        <v>11452</v>
+      </c>
+      <c r="D170" s="2">
+        <v>8.93</v>
+      </c>
+      <c r="E170" s="2">
+        <v>13</v>
+      </c>
+      <c r="F170" s="2">
+        <v>678</v>
+      </c>
+      <c r="G170" s="2">
+        <v>351</v>
+      </c>
+      <c r="H170" s="2">
+        <v>15</v>
+      </c>
+      <c r="I170" s="2">
+        <v>19</v>
+      </c>
+      <c r="J170" s="2">
+        <v>2009</v>
+      </c>
+      <c r="K170" t="str">
+        <f t="shared" si="12"/>
+        <v>Yes</v>
+      </c>
+      <c r="L170" t="str">
+        <f t="shared" si="13"/>
+        <v>Yes</v>
+      </c>
+      <c r="M170" t="str">
+        <f t="shared" si="14"/>
+        <v>No</v>
+      </c>
+      <c r="N170" t="str">
+        <f t="shared" si="15"/>
+        <v>No</v>
+      </c>
+      <c r="O170" t="str">
+        <f t="shared" si="11"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="171" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A171" s="1">
+        <v>43148</v>
+      </c>
+      <c r="B171" s="2">
+        <v>3969</v>
+      </c>
+      <c r="C171" s="2">
+        <v>15867</v>
+      </c>
+      <c r="D171" s="2">
+        <v>12.38</v>
+      </c>
+      <c r="E171" s="2">
+        <v>25</v>
+      </c>
+      <c r="F171" s="2">
+        <v>574</v>
+      </c>
+      <c r="G171" s="2">
+        <v>365</v>
+      </c>
+      <c r="H171" s="2">
+        <v>64</v>
+      </c>
+      <c r="I171" s="2">
+        <v>22</v>
+      </c>
+      <c r="J171" s="2">
+        <v>2463</v>
+      </c>
+      <c r="K171" t="str">
+        <f t="shared" si="12"/>
+        <v>Yes</v>
+      </c>
+      <c r="L171" t="str">
+        <f t="shared" si="13"/>
+        <v>Yes</v>
+      </c>
+      <c r="M171" t="str">
+        <f t="shared" si="14"/>
+        <v>No</v>
+      </c>
+      <c r="N171" t="str">
+        <f t="shared" si="15"/>
+        <v>No</v>
+      </c>
+      <c r="O171" t="str">
+        <f t="shared" si="11"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="172" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A172" s="1">
+        <v>43149</v>
+      </c>
+      <c r="B172" s="2">
+        <v>4594</v>
+      </c>
+      <c r="C172" s="2">
+        <v>13462</v>
+      </c>
+      <c r="D172" s="2">
+        <v>10.24</v>
+      </c>
+      <c r="E172" s="2">
+        <v>23</v>
+      </c>
+      <c r="F172" s="2">
+        <v>543</v>
+      </c>
+      <c r="G172" s="2">
+        <v>344</v>
+      </c>
+      <c r="H172" s="2">
+        <v>59</v>
+      </c>
+      <c r="I172" s="2">
+        <v>78</v>
+      </c>
+      <c r="J172" s="2">
+        <v>3098</v>
+      </c>
+      <c r="K172" t="str">
+        <f t="shared" si="12"/>
+        <v>Yes</v>
+      </c>
+      <c r="L172" t="str">
+        <f t="shared" si="13"/>
+        <v>Yes</v>
+      </c>
+      <c r="M172" t="str">
+        <f t="shared" si="14"/>
+        <v>Yes</v>
+      </c>
+      <c r="N172" t="str">
+        <f t="shared" si="15"/>
+        <v>No</v>
+      </c>
+      <c r="O172" t="str">
+        <f t="shared" si="11"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="173" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A173" s="1">
+        <v>43150</v>
+      </c>
+      <c r="B173" s="2">
+        <v>3636</v>
+      </c>
+      <c r="C173" s="2">
+        <v>8309</v>
+      </c>
+      <c r="D173" s="2">
+        <v>6.29</v>
+      </c>
+      <c r="E173" s="2">
+        <v>15</v>
+      </c>
+      <c r="F173" s="2">
+        <v>711</v>
+      </c>
+      <c r="G173" s="2">
+        <v>257</v>
+      </c>
+      <c r="H173" s="2">
+        <v>27</v>
+      </c>
+      <c r="I173" s="2">
+        <v>59</v>
+      </c>
+      <c r="J173" s="2">
+        <v>1962</v>
+      </c>
+      <c r="K173" t="str">
+        <f t="shared" si="12"/>
+        <v>Yes</v>
+      </c>
+      <c r="L173" t="str">
+        <f t="shared" si="13"/>
+        <v>Yes</v>
+      </c>
+      <c r="M173" t="str">
+        <f t="shared" si="14"/>
+        <v>Yes</v>
+      </c>
+      <c r="N173" t="str">
+        <f t="shared" si="15"/>
+        <v>No</v>
+      </c>
+      <c r="O173" t="str">
+        <f t="shared" si="11"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="174" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A174" s="1">
+        <v>43151</v>
+      </c>
+      <c r="B174" s="2">
+        <v>3798</v>
+      </c>
+      <c r="C174" s="2">
+        <v>8373</v>
+      </c>
+      <c r="D174" s="2">
+        <v>6.19</v>
+      </c>
+      <c r="E174" s="2">
+        <v>10</v>
+      </c>
+      <c r="F174" s="2">
+        <v>721</v>
+      </c>
+      <c r="G174" s="2">
+        <v>212</v>
+      </c>
+      <c r="H174" s="2">
+        <v>33</v>
+      </c>
+      <c r="I174" s="2">
+        <v>77</v>
+      </c>
+      <c r="J174" s="2">
+        <v>2078</v>
+      </c>
+      <c r="K174" t="str">
+        <f t="shared" si="12"/>
+        <v>Yes</v>
+      </c>
+      <c r="L174" t="str">
+        <f t="shared" si="13"/>
+        <v>Yes</v>
+      </c>
+      <c r="M174" t="str">
+        <f t="shared" si="14"/>
+        <v>Yes</v>
+      </c>
+      <c r="N174" t="str">
+        <f t="shared" si="15"/>
+        <v>No</v>
+      </c>
+      <c r="O174" t="str">
+        <f t="shared" ref="O174:O182" si="16">IF(D174&gt;5,"Yes","No")</f>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="175" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A175" s="1">
+        <v>43152</v>
+      </c>
+      <c r="B175" s="2">
+        <v>3093</v>
+      </c>
+      <c r="C175" s="2">
+        <v>7791</v>
+      </c>
+      <c r="D175" s="2">
+        <v>6.08</v>
+      </c>
+      <c r="E175" s="2">
+        <v>13</v>
+      </c>
+      <c r="F175" s="2">
+        <v>789</v>
+      </c>
+      <c r="G175" s="2">
+        <v>286</v>
+      </c>
+      <c r="H175" s="2">
+        <v>0</v>
+      </c>
+      <c r="I175" s="2">
+        <v>0</v>
+      </c>
+      <c r="J175" s="2">
+        <v>1321</v>
+      </c>
+      <c r="K175" t="str">
+        <f t="shared" si="12"/>
+        <v>No</v>
+      </c>
+      <c r="L175" t="str">
+        <f t="shared" si="13"/>
+        <v>No</v>
+      </c>
+      <c r="M175" t="str">
+        <f t="shared" si="14"/>
+        <v>No</v>
+      </c>
+      <c r="N175" t="str">
+        <f t="shared" si="15"/>
+        <v>Yes</v>
+      </c>
+      <c r="O175" t="str">
+        <f t="shared" si="16"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="176" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A176" s="1">
+        <v>43153</v>
+      </c>
+      <c r="B176" s="2">
+        <v>3704</v>
+      </c>
+      <c r="C176" s="2">
+        <v>9824</v>
+      </c>
+      <c r="D176" s="2">
+        <v>7.38</v>
+      </c>
+      <c r="E176" s="2">
+        <v>9</v>
+      </c>
+      <c r="F176" s="2">
+        <v>706</v>
+      </c>
+      <c r="G176" s="2">
+        <v>308</v>
+      </c>
+      <c r="H176" s="2">
+        <v>24</v>
+      </c>
+      <c r="I176" s="2">
+        <v>28</v>
+      </c>
+      <c r="J176" s="2">
+        <v>1999</v>
+      </c>
+      <c r="K176" t="str">
+        <f t="shared" si="12"/>
+        <v>Yes</v>
+      </c>
+      <c r="L176" t="str">
+        <f t="shared" si="13"/>
+        <v>Yes</v>
+      </c>
+      <c r="M176" t="str">
+        <f t="shared" si="14"/>
+        <v>No</v>
+      </c>
+      <c r="N176" t="str">
+        <f t="shared" si="15"/>
+        <v>No</v>
+      </c>
+      <c r="O176" t="str">
+        <f t="shared" si="16"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="177" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A177" s="1">
+        <v>43154</v>
+      </c>
+      <c r="B177" s="2">
+        <v>3596</v>
+      </c>
+      <c r="C177" s="2">
+        <v>13194</v>
+      </c>
+      <c r="D177" s="2">
+        <v>10.29</v>
+      </c>
+      <c r="E177" s="2">
+        <v>19</v>
+      </c>
+      <c r="F177" s="2">
+        <v>643</v>
+      </c>
+      <c r="G177" s="2">
+        <v>302</v>
+      </c>
+      <c r="H177" s="2">
+        <v>14</v>
+      </c>
+      <c r="I177" s="2">
+        <v>32</v>
+      </c>
+      <c r="J177" s="2">
+        <v>1913</v>
+      </c>
+      <c r="K177" t="str">
+        <f t="shared" si="12"/>
+        <v>Yes</v>
+      </c>
+      <c r="L177" t="str">
+        <f t="shared" si="13"/>
+        <v>Yes</v>
+      </c>
+      <c r="M177" t="str">
+        <f t="shared" si="14"/>
+        <v>Yes</v>
+      </c>
+      <c r="N177" t="str">
+        <f t="shared" si="15"/>
+        <v>No</v>
+      </c>
+      <c r="O177" t="str">
+        <f t="shared" si="16"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="178" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A178" s="1">
+        <v>43155</v>
+      </c>
+      <c r="B178" s="2">
+        <v>5110</v>
+      </c>
+      <c r="C178" s="2">
+        <v>13202</v>
+      </c>
+      <c r="D178" s="2">
+        <v>10.09</v>
+      </c>
+      <c r="E178" s="2">
+        <v>20</v>
+      </c>
+      <c r="F178" s="2">
+        <v>398</v>
+      </c>
+      <c r="G178" s="2">
+        <v>321</v>
+      </c>
+      <c r="H178" s="2">
+        <v>107</v>
+      </c>
+      <c r="I178" s="2">
+        <v>125</v>
+      </c>
+      <c r="J178" s="2">
+        <v>3746</v>
+      </c>
+      <c r="K178" t="str">
+        <f t="shared" si="12"/>
+        <v>Yes</v>
+      </c>
+      <c r="L178" t="str">
+        <f t="shared" si="13"/>
+        <v>Yes</v>
+      </c>
+      <c r="M178" t="str">
+        <f t="shared" si="14"/>
+        <v>Yes</v>
+      </c>
+      <c r="N178" t="str">
+        <f t="shared" si="15"/>
+        <v>No</v>
+      </c>
+      <c r="O178" t="str">
+        <f t="shared" si="16"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="179" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A179" s="1">
+        <v>43156</v>
+      </c>
+      <c r="B179" s="2">
+        <v>4171</v>
+      </c>
+      <c r="C179" s="2">
+        <v>10451</v>
+      </c>
+      <c r="D179" s="2">
+        <v>8.15</v>
+      </c>
+      <c r="E179" s="2">
+        <v>14</v>
+      </c>
+      <c r="F179" s="2">
+        <v>677</v>
+      </c>
+      <c r="G179" s="2">
+        <v>300</v>
+      </c>
+      <c r="H179" s="2">
+        <v>42</v>
+      </c>
+      <c r="I179" s="2">
+        <v>75</v>
+      </c>
+      <c r="J179" s="2">
+        <v>2549</v>
+      </c>
+      <c r="K179" t="str">
+        <f t="shared" si="12"/>
+        <v>Yes</v>
+      </c>
+      <c r="L179" t="str">
+        <f t="shared" si="13"/>
+        <v>Yes</v>
+      </c>
+      <c r="M179" t="str">
+        <f t="shared" si="14"/>
+        <v>Yes</v>
+      </c>
+      <c r="N179" t="str">
+        <f t="shared" si="15"/>
+        <v>No</v>
+      </c>
+      <c r="O179" t="str">
+        <f t="shared" si="16"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="180" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A180" s="1">
+        <v>43157</v>
+      </c>
+      <c r="B180" s="2">
+        <v>3387</v>
+      </c>
+      <c r="C180" s="2">
+        <v>7661</v>
+      </c>
+      <c r="D180" s="2">
+        <v>5.75</v>
+      </c>
+      <c r="E180" s="2">
+        <v>11</v>
+      </c>
+      <c r="F180" s="2">
+        <v>717</v>
+      </c>
+      <c r="G180" s="2">
+        <v>244</v>
+      </c>
+      <c r="H180" s="2">
+        <v>18</v>
+      </c>
+      <c r="I180" s="2">
+        <v>32</v>
+      </c>
+      <c r="J180" s="2">
+        <v>1599</v>
+      </c>
+      <c r="K180" t="str">
+        <f t="shared" si="12"/>
+        <v>No</v>
+      </c>
+      <c r="L180" t="str">
+        <f t="shared" si="13"/>
+        <v>No</v>
+      </c>
+      <c r="M180" t="str">
+        <f t="shared" si="14"/>
+        <v>Yes</v>
+      </c>
+      <c r="N180" t="str">
+        <f t="shared" si="15"/>
+        <v>No</v>
+      </c>
+      <c r="O180" t="str">
+        <f t="shared" si="16"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="181" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A181" s="1">
+        <v>43158</v>
+      </c>
+      <c r="B181" s="2">
+        <v>3008</v>
+      </c>
+      <c r="C181" s="2">
+        <v>6607</v>
+      </c>
+      <c r="D181" s="2">
+        <v>5.15</v>
+      </c>
+      <c r="E181" s="2">
+        <v>6</v>
+      </c>
+      <c r="F181" s="2">
+        <v>727</v>
+      </c>
+      <c r="G181" s="2">
+        <v>296</v>
+      </c>
+      <c r="H181" s="2">
+        <v>0</v>
+      </c>
+      <c r="I181" s="2">
+        <v>0</v>
+      </c>
+      <c r="J181" s="2">
+        <v>1282</v>
+      </c>
+      <c r="K181" t="str">
+        <f t="shared" si="12"/>
+        <v>No</v>
+      </c>
+      <c r="L181" t="str">
+        <f t="shared" si="13"/>
+        <v>No</v>
+      </c>
+      <c r="M181" t="str">
+        <f t="shared" si="14"/>
+        <v>No</v>
+      </c>
+      <c r="N181" t="str">
+        <f t="shared" si="15"/>
+        <v>Yes</v>
+      </c>
+      <c r="O181" t="str">
+        <f t="shared" si="16"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="182" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A182" s="1">
+        <v>43159</v>
+      </c>
+      <c r="B182" s="2">
+        <v>4129</v>
+      </c>
+      <c r="C182" s="2">
+        <v>11370</v>
+      </c>
+      <c r="D182" s="2">
+        <v>8.5399999999999991</v>
+      </c>
+      <c r="E182" s="2">
+        <v>17</v>
+      </c>
+      <c r="F182" s="2">
+        <v>629</v>
+      </c>
+      <c r="G182" s="2">
+        <v>283</v>
+      </c>
+      <c r="H182" s="2">
+        <v>32</v>
+      </c>
+      <c r="I182" s="2">
+        <v>84</v>
+      </c>
+      <c r="J182" s="2">
+        <v>2516</v>
+      </c>
+      <c r="K182" t="str">
+        <f t="shared" si="12"/>
+        <v>Yes</v>
+      </c>
+      <c r="L182" t="str">
+        <f t="shared" si="13"/>
+        <v>Yes</v>
+      </c>
+      <c r="M182" t="str">
+        <f t="shared" si="14"/>
+        <v>Yes</v>
+      </c>
+      <c r="N182" t="str">
+        <f t="shared" si="15"/>
+        <v>No</v>
+      </c>
+      <c r="O182" t="str">
+        <f t="shared" si="16"/>
         <v>Yes</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updating TotalExercise file to include 31/03/2018 date
</commit_message>
<xml_diff>
--- a/datasets/TotalExercise.xlsx
+++ b/datasets/TotalExercise.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Will\Documents\Data Science\My Projects\My Data Project\mydata\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12AB10F9-4783-452F-AE8F-411BC46F9B80}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6867F0E-93A6-423E-9141-C4D7F00EB7AA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="11800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TotalExercise" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
@@ -74,7 +74,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -213,6 +213,16 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="33">
@@ -512,7 +522,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="44">
+  <cellStyleXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -557,8 +567,9 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -566,8 +577,9 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="43" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="20" fillId="0" borderId="0" xfId="44" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="44">
+  <cellStyles count="45">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -607,6 +619,7 @@
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="42" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
+    <cellStyle name="Normal 3" xfId="44" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
@@ -923,10 +936,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O212"/>
+  <dimension ref="A1:O213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A213" workbookViewId="0">
-      <selection activeCell="C209" sqref="C209"/>
+    <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
+      <selection activeCell="D121" sqref="D121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9984,7 +9997,7 @@
         <v>No</v>
       </c>
       <c r="O174" t="str">
-        <f t="shared" ref="O174:O212" si="16">IF(D174&gt;5,"Yes","No")</f>
+        <f t="shared" ref="O174:O213" si="16">IF(D174&gt;5,"Yes","No")</f>
         <v>Yes</v>
       </c>
     </row>
@@ -11060,19 +11073,19 @@
         <v>1954</v>
       </c>
       <c r="K195" t="str">
-        <f t="shared" ref="K195:K212" si="17">IF(C195&gt;8000,"Yes","No")</f>
+        <f t="shared" ref="K195:K213" si="17">IF(C195&gt;8000,"Yes","No")</f>
         <v>Yes</v>
       </c>
       <c r="L195" t="str">
-        <f t="shared" ref="L195:L212" si="18">IF(B195&gt;3400,"Yes","No")</f>
+        <f t="shared" ref="L195:L213" si="18">IF(B195&gt;3400,"Yes","No")</f>
         <v>Yes</v>
       </c>
       <c r="M195" t="str">
-        <f t="shared" ref="M195:M212" si="19">IF(I195&gt;30,"Yes","No")</f>
+        <f t="shared" ref="M195:M213" si="19">IF(I195&gt;30,"Yes","No")</f>
         <v>Yes</v>
       </c>
       <c r="N195" t="str">
-        <f t="shared" ref="N195:N212" si="20">IF(I195+H195&lt;30,"Yes","No")</f>
+        <f t="shared" ref="N195:N213" si="20">IF(I195+H195&lt;30,"Yes","No")</f>
         <v>No</v>
       </c>
       <c r="O195" t="str">
@@ -11960,6 +11973,58 @@
         <v>Yes</v>
       </c>
       <c r="O212" t="str">
+        <f t="shared" si="16"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="213" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A213" s="1">
+        <v>43190</v>
+      </c>
+      <c r="B213" s="7">
+        <v>2934</v>
+      </c>
+      <c r="C213" s="7">
+        <v>7461</v>
+      </c>
+      <c r="D213" s="7">
+        <v>5.82</v>
+      </c>
+      <c r="E213" s="7">
+        <v>11</v>
+      </c>
+      <c r="F213" s="7">
+        <v>691</v>
+      </c>
+      <c r="G213" s="7">
+        <v>302</v>
+      </c>
+      <c r="H213" s="7">
+        <v>0</v>
+      </c>
+      <c r="I213" s="7">
+        <v>0</v>
+      </c>
+      <c r="J213" s="7">
+        <v>1274</v>
+      </c>
+      <c r="K213" t="str">
+        <f t="shared" si="17"/>
+        <v>No</v>
+      </c>
+      <c r="L213" t="str">
+        <f t="shared" si="18"/>
+        <v>No</v>
+      </c>
+      <c r="M213" t="str">
+        <f t="shared" si="19"/>
+        <v>No</v>
+      </c>
+      <c r="N213" t="str">
+        <f t="shared" si="20"/>
+        <v>Yes</v>
+      </c>
+      <c r="O213" t="str">
         <f t="shared" si="16"/>
         <v>Yes</v>
       </c>

</xml_diff>

<commit_message>
Updating TotalExercise file 01/05/2018
</commit_message>
<xml_diff>
--- a/datasets/TotalExercise.xlsx
+++ b/datasets/TotalExercise.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Will\Documents\Data Science\My Projects\My Data Project\mydata\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6867F0E-93A6-423E-9141-C4D7F00EB7AA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB8823D9-6F38-452E-B162-3BCB50613DB4}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="11800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -569,7 +569,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -578,6 +578,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="43" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="20" fillId="0" borderId="0" xfId="44" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="19" fillId="0" borderId="0" xfId="44" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="45">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -936,10 +937,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O213"/>
+  <dimension ref="A1:O243"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
-      <selection activeCell="D121" sqref="D121"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L237" sqref="L237"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9997,7 +9998,7 @@
         <v>No</v>
       </c>
       <c r="O174" t="str">
-        <f t="shared" ref="O174:O213" si="16">IF(D174&gt;5,"Yes","No")</f>
+        <f t="shared" ref="O174:O237" si="16">IF(D174&gt;5,"Yes","No")</f>
         <v>Yes</v>
       </c>
     </row>
@@ -11073,19 +11074,19 @@
         <v>1954</v>
       </c>
       <c r="K195" t="str">
-        <f t="shared" ref="K195:K213" si="17">IF(C195&gt;8000,"Yes","No")</f>
+        <f t="shared" ref="K195:K243" si="17">IF(C195&gt;8000,"Yes","No")</f>
         <v>Yes</v>
       </c>
       <c r="L195" t="str">
-        <f t="shared" ref="L195:L213" si="18">IF(B195&gt;3400,"Yes","No")</f>
+        <f t="shared" ref="L195:L243" si="18">IF(B195&gt;3400,"Yes","No")</f>
         <v>Yes</v>
       </c>
       <c r="M195" t="str">
-        <f t="shared" ref="M195:M213" si="19">IF(I195&gt;30,"Yes","No")</f>
+        <f t="shared" ref="M195:M243" si="19">IF(I195&gt;30,"Yes","No")</f>
         <v>Yes</v>
       </c>
       <c r="N195" t="str">
-        <f t="shared" ref="N195:N213" si="20">IF(I195+H195&lt;30,"Yes","No")</f>
+        <f t="shared" ref="N195:N243" si="20">IF(I195+H195&lt;30,"Yes","No")</f>
         <v>No</v>
       </c>
       <c r="O195" t="str">
@@ -12026,6 +12027,1566 @@
       </c>
       <c r="O213" t="str">
         <f t="shared" si="16"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="214" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A214" s="1">
+        <v>43191</v>
+      </c>
+      <c r="B214" s="8">
+        <v>3582</v>
+      </c>
+      <c r="C214" s="8">
+        <v>8001</v>
+      </c>
+      <c r="D214" s="8">
+        <v>6</v>
+      </c>
+      <c r="E214" s="8">
+        <v>15</v>
+      </c>
+      <c r="F214" s="8">
+        <v>730</v>
+      </c>
+      <c r="G214" s="8">
+        <v>244</v>
+      </c>
+      <c r="H214" s="8">
+        <v>19</v>
+      </c>
+      <c r="I214" s="8">
+        <v>45</v>
+      </c>
+      <c r="J214" s="8">
+        <v>1751</v>
+      </c>
+      <c r="K214" t="str">
+        <f t="shared" si="17"/>
+        <v>Yes</v>
+      </c>
+      <c r="L214" t="str">
+        <f t="shared" si="18"/>
+        <v>Yes</v>
+      </c>
+      <c r="M214" t="str">
+        <f t="shared" si="19"/>
+        <v>Yes</v>
+      </c>
+      <c r="N214" t="str">
+        <f t="shared" si="20"/>
+        <v>No</v>
+      </c>
+      <c r="O214" t="str">
+        <f t="shared" si="16"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="215" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A215" s="1">
+        <v>43192</v>
+      </c>
+      <c r="B215" s="8">
+        <v>3753</v>
+      </c>
+      <c r="C215" s="8">
+        <v>10213</v>
+      </c>
+      <c r="D215" s="8">
+        <v>7.56</v>
+      </c>
+      <c r="E215" s="8">
+        <v>11</v>
+      </c>
+      <c r="F215" s="8">
+        <v>674</v>
+      </c>
+      <c r="G215" s="8">
+        <v>264</v>
+      </c>
+      <c r="H215" s="8">
+        <v>23</v>
+      </c>
+      <c r="I215" s="8">
+        <v>61</v>
+      </c>
+      <c r="J215" s="8">
+        <v>2116</v>
+      </c>
+      <c r="K215" t="str">
+        <f t="shared" si="17"/>
+        <v>Yes</v>
+      </c>
+      <c r="L215" t="str">
+        <f t="shared" si="18"/>
+        <v>Yes</v>
+      </c>
+      <c r="M215" t="str">
+        <f t="shared" si="19"/>
+        <v>Yes</v>
+      </c>
+      <c r="N215" t="str">
+        <f t="shared" si="20"/>
+        <v>No</v>
+      </c>
+      <c r="O215" t="str">
+        <f t="shared" si="16"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="216" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A216" s="1">
+        <v>43193</v>
+      </c>
+      <c r="B216" s="8">
+        <v>2940</v>
+      </c>
+      <c r="C216" s="8">
+        <v>7319</v>
+      </c>
+      <c r="D216" s="8">
+        <v>5.71</v>
+      </c>
+      <c r="E216" s="8">
+        <v>10</v>
+      </c>
+      <c r="F216" s="8">
+        <v>769</v>
+      </c>
+      <c r="G216" s="8">
+        <v>289</v>
+      </c>
+      <c r="H216" s="8">
+        <v>0</v>
+      </c>
+      <c r="I216" s="8">
+        <v>0</v>
+      </c>
+      <c r="J216" s="8">
+        <v>1244</v>
+      </c>
+      <c r="K216" t="str">
+        <f t="shared" si="17"/>
+        <v>No</v>
+      </c>
+      <c r="L216" t="str">
+        <f t="shared" si="18"/>
+        <v>No</v>
+      </c>
+      <c r="M216" t="str">
+        <f t="shared" si="19"/>
+        <v>No</v>
+      </c>
+      <c r="N216" t="str">
+        <f t="shared" si="20"/>
+        <v>Yes</v>
+      </c>
+      <c r="O216" t="str">
+        <f t="shared" si="16"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="217" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A217" s="1">
+        <v>43194</v>
+      </c>
+      <c r="B217" s="8">
+        <v>3838</v>
+      </c>
+      <c r="C217" s="8">
+        <v>11694</v>
+      </c>
+      <c r="D217" s="8">
+        <v>8.9</v>
+      </c>
+      <c r="E217" s="8">
+        <v>17</v>
+      </c>
+      <c r="F217" s="8">
+        <v>1113</v>
+      </c>
+      <c r="G217" s="8">
+        <v>242</v>
+      </c>
+      <c r="H217" s="8">
+        <v>9</v>
+      </c>
+      <c r="I217" s="8">
+        <v>76</v>
+      </c>
+      <c r="J217" s="8">
+        <v>2121</v>
+      </c>
+      <c r="K217" t="str">
+        <f t="shared" si="17"/>
+        <v>Yes</v>
+      </c>
+      <c r="L217" t="str">
+        <f t="shared" si="18"/>
+        <v>Yes</v>
+      </c>
+      <c r="M217" t="str">
+        <f t="shared" si="19"/>
+        <v>Yes</v>
+      </c>
+      <c r="N217" t="str">
+        <f t="shared" si="20"/>
+        <v>No</v>
+      </c>
+      <c r="O217" t="str">
+        <f t="shared" si="16"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="218" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A218" s="1">
+        <v>43195</v>
+      </c>
+      <c r="B218" s="8">
+        <v>3279</v>
+      </c>
+      <c r="C218" s="8">
+        <v>8322</v>
+      </c>
+      <c r="D218" s="8">
+        <v>6.39</v>
+      </c>
+      <c r="E218" s="8">
+        <v>18</v>
+      </c>
+      <c r="F218" s="8">
+        <v>879</v>
+      </c>
+      <c r="G218" s="8">
+        <v>259</v>
+      </c>
+      <c r="H218" s="8">
+        <v>22</v>
+      </c>
+      <c r="I218" s="8">
+        <v>29</v>
+      </c>
+      <c r="J218" s="8">
+        <v>1609</v>
+      </c>
+      <c r="K218" t="str">
+        <f t="shared" si="17"/>
+        <v>Yes</v>
+      </c>
+      <c r="L218" t="str">
+        <f t="shared" si="18"/>
+        <v>No</v>
+      </c>
+      <c r="M218" t="str">
+        <f t="shared" si="19"/>
+        <v>No</v>
+      </c>
+      <c r="N218" t="str">
+        <f t="shared" si="20"/>
+        <v>No</v>
+      </c>
+      <c r="O218" t="str">
+        <f t="shared" si="16"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="219" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A219" s="1">
+        <v>43196</v>
+      </c>
+      <c r="B219" s="8">
+        <v>2887</v>
+      </c>
+      <c r="C219" s="8">
+        <v>6694</v>
+      </c>
+      <c r="D219" s="8">
+        <v>5.22</v>
+      </c>
+      <c r="E219" s="8">
+        <v>15</v>
+      </c>
+      <c r="F219" s="8">
+        <v>817</v>
+      </c>
+      <c r="G219" s="8">
+        <v>228</v>
+      </c>
+      <c r="H219" s="8">
+        <v>1</v>
+      </c>
+      <c r="I219" s="8">
+        <v>7</v>
+      </c>
+      <c r="J219" s="8">
+        <v>1094</v>
+      </c>
+      <c r="K219" t="str">
+        <f t="shared" si="17"/>
+        <v>No</v>
+      </c>
+      <c r="L219" t="str">
+        <f t="shared" si="18"/>
+        <v>No</v>
+      </c>
+      <c r="M219" t="str">
+        <f t="shared" si="19"/>
+        <v>No</v>
+      </c>
+      <c r="N219" t="str">
+        <f t="shared" si="20"/>
+        <v>Yes</v>
+      </c>
+      <c r="O219" t="str">
+        <f t="shared" si="16"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="220" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A220" s="1">
+        <v>43197</v>
+      </c>
+      <c r="B220" s="8">
+        <v>3844</v>
+      </c>
+      <c r="C220" s="8">
+        <v>10909</v>
+      </c>
+      <c r="D220" s="8">
+        <v>8.31</v>
+      </c>
+      <c r="E220" s="8">
+        <v>19</v>
+      </c>
+      <c r="F220" s="8">
+        <v>575</v>
+      </c>
+      <c r="G220" s="8">
+        <v>385</v>
+      </c>
+      <c r="H220" s="8">
+        <v>30</v>
+      </c>
+      <c r="I220" s="8">
+        <v>5</v>
+      </c>
+      <c r="J220" s="8">
+        <v>2247</v>
+      </c>
+      <c r="K220" t="str">
+        <f t="shared" si="17"/>
+        <v>Yes</v>
+      </c>
+      <c r="L220" t="str">
+        <f t="shared" si="18"/>
+        <v>Yes</v>
+      </c>
+      <c r="M220" t="str">
+        <f t="shared" si="19"/>
+        <v>No</v>
+      </c>
+      <c r="N220" t="str">
+        <f t="shared" si="20"/>
+        <v>No</v>
+      </c>
+      <c r="O220" t="str">
+        <f t="shared" si="16"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="221" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A221" s="1">
+        <v>43198</v>
+      </c>
+      <c r="B221" s="8">
+        <v>3739</v>
+      </c>
+      <c r="C221" s="8">
+        <v>11277</v>
+      </c>
+      <c r="D221" s="8">
+        <v>8.4700000000000006</v>
+      </c>
+      <c r="E221" s="8">
+        <v>7</v>
+      </c>
+      <c r="F221" s="8">
+        <v>677</v>
+      </c>
+      <c r="G221" s="8">
+        <v>337</v>
+      </c>
+      <c r="H221" s="8">
+        <v>18</v>
+      </c>
+      <c r="I221" s="8">
+        <v>49</v>
+      </c>
+      <c r="J221" s="8">
+        <v>2177</v>
+      </c>
+      <c r="K221" t="str">
+        <f t="shared" si="17"/>
+        <v>Yes</v>
+      </c>
+      <c r="L221" t="str">
+        <f t="shared" si="18"/>
+        <v>Yes</v>
+      </c>
+      <c r="M221" t="str">
+        <f t="shared" si="19"/>
+        <v>Yes</v>
+      </c>
+      <c r="N221" t="str">
+        <f t="shared" si="20"/>
+        <v>No</v>
+      </c>
+      <c r="O221" t="str">
+        <f t="shared" si="16"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="222" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A222" s="1">
+        <v>43199</v>
+      </c>
+      <c r="B222" s="8">
+        <v>2804</v>
+      </c>
+      <c r="C222" s="8">
+        <v>5519</v>
+      </c>
+      <c r="D222" s="8">
+        <v>4.3</v>
+      </c>
+      <c r="E222" s="8">
+        <v>11</v>
+      </c>
+      <c r="F222" s="8">
+        <v>776</v>
+      </c>
+      <c r="G222" s="8">
+        <v>224</v>
+      </c>
+      <c r="H222" s="8">
+        <v>0</v>
+      </c>
+      <c r="I222" s="8">
+        <v>0</v>
+      </c>
+      <c r="J222" s="8">
+        <v>990</v>
+      </c>
+      <c r="K222" t="str">
+        <f t="shared" si="17"/>
+        <v>No</v>
+      </c>
+      <c r="L222" t="str">
+        <f t="shared" si="18"/>
+        <v>No</v>
+      </c>
+      <c r="M222" t="str">
+        <f t="shared" si="19"/>
+        <v>No</v>
+      </c>
+      <c r="N222" t="str">
+        <f t="shared" si="20"/>
+        <v>Yes</v>
+      </c>
+      <c r="O222" t="str">
+        <f t="shared" si="16"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="223" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A223" s="1">
+        <v>43200</v>
+      </c>
+      <c r="B223" s="8">
+        <v>3671</v>
+      </c>
+      <c r="C223" s="8">
+        <v>9550</v>
+      </c>
+      <c r="D223" s="8">
+        <v>7.21</v>
+      </c>
+      <c r="E223" s="8">
+        <v>18</v>
+      </c>
+      <c r="F223" s="8">
+        <v>763</v>
+      </c>
+      <c r="G223" s="8">
+        <v>225</v>
+      </c>
+      <c r="H223" s="8">
+        <v>19</v>
+      </c>
+      <c r="I223" s="8">
+        <v>61</v>
+      </c>
+      <c r="J223" s="8">
+        <v>1892</v>
+      </c>
+      <c r="K223" t="str">
+        <f t="shared" si="17"/>
+        <v>Yes</v>
+      </c>
+      <c r="L223" t="str">
+        <f t="shared" si="18"/>
+        <v>Yes</v>
+      </c>
+      <c r="M223" t="str">
+        <f t="shared" si="19"/>
+        <v>Yes</v>
+      </c>
+      <c r="N223" t="str">
+        <f t="shared" si="20"/>
+        <v>No</v>
+      </c>
+      <c r="O223" t="str">
+        <f t="shared" si="16"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="224" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A224" s="1">
+        <v>43201</v>
+      </c>
+      <c r="B224" s="8">
+        <v>2795</v>
+      </c>
+      <c r="C224" s="8">
+        <v>5718</v>
+      </c>
+      <c r="D224" s="8">
+        <v>4.46</v>
+      </c>
+      <c r="E224" s="8">
+        <v>14</v>
+      </c>
+      <c r="F224" s="8">
+        <v>726</v>
+      </c>
+      <c r="G224" s="8">
+        <v>243</v>
+      </c>
+      <c r="H224" s="8">
+        <v>0</v>
+      </c>
+      <c r="I224" s="8">
+        <v>0</v>
+      </c>
+      <c r="J224" s="8">
+        <v>1022</v>
+      </c>
+      <c r="K224" t="str">
+        <f t="shared" si="17"/>
+        <v>No</v>
+      </c>
+      <c r="L224" t="str">
+        <f t="shared" si="18"/>
+        <v>No</v>
+      </c>
+      <c r="M224" t="str">
+        <f t="shared" si="19"/>
+        <v>No</v>
+      </c>
+      <c r="N224" t="str">
+        <f t="shared" si="20"/>
+        <v>Yes</v>
+      </c>
+      <c r="O224" t="str">
+        <f t="shared" si="16"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="225" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A225" s="1">
+        <v>43202</v>
+      </c>
+      <c r="B225" s="8">
+        <v>2999</v>
+      </c>
+      <c r="C225" s="8">
+        <v>6793</v>
+      </c>
+      <c r="D225" s="8">
+        <v>5.3</v>
+      </c>
+      <c r="E225" s="8">
+        <v>25</v>
+      </c>
+      <c r="F225" s="8">
+        <v>822</v>
+      </c>
+      <c r="G225" s="8">
+        <v>288</v>
+      </c>
+      <c r="H225" s="8">
+        <v>0</v>
+      </c>
+      <c r="I225" s="8">
+        <v>0</v>
+      </c>
+      <c r="J225" s="8">
+        <v>1263</v>
+      </c>
+      <c r="K225" t="str">
+        <f t="shared" si="17"/>
+        <v>No</v>
+      </c>
+      <c r="L225" t="str">
+        <f t="shared" si="18"/>
+        <v>No</v>
+      </c>
+      <c r="M225" t="str">
+        <f t="shared" si="19"/>
+        <v>No</v>
+      </c>
+      <c r="N225" t="str">
+        <f t="shared" si="20"/>
+        <v>Yes</v>
+      </c>
+      <c r="O225" t="str">
+        <f t="shared" si="16"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="226" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A226" s="1">
+        <v>43203</v>
+      </c>
+      <c r="B226" s="8">
+        <v>3753</v>
+      </c>
+      <c r="C226" s="8">
+        <v>10787</v>
+      </c>
+      <c r="D226" s="8">
+        <v>8.33</v>
+      </c>
+      <c r="E226" s="8">
+        <v>23</v>
+      </c>
+      <c r="F226" s="8">
+        <v>733</v>
+      </c>
+      <c r="G226" s="8">
+        <v>259</v>
+      </c>
+      <c r="H226" s="8">
+        <v>15</v>
+      </c>
+      <c r="I226" s="8">
+        <v>44</v>
+      </c>
+      <c r="J226" s="8">
+        <v>1960</v>
+      </c>
+      <c r="K226" t="str">
+        <f t="shared" si="17"/>
+        <v>Yes</v>
+      </c>
+      <c r="L226" t="str">
+        <f t="shared" si="18"/>
+        <v>Yes</v>
+      </c>
+      <c r="M226" t="str">
+        <f t="shared" si="19"/>
+        <v>Yes</v>
+      </c>
+      <c r="N226" t="str">
+        <f t="shared" si="20"/>
+        <v>No</v>
+      </c>
+      <c r="O226" t="str">
+        <f t="shared" si="16"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="227" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A227" s="1">
+        <v>43204</v>
+      </c>
+      <c r="B227" s="8">
+        <v>3099</v>
+      </c>
+      <c r="C227" s="8">
+        <v>8364</v>
+      </c>
+      <c r="D227" s="8">
+        <v>6.52</v>
+      </c>
+      <c r="E227" s="8">
+        <v>9</v>
+      </c>
+      <c r="F227" s="8">
+        <v>653</v>
+      </c>
+      <c r="G227" s="8">
+        <v>316</v>
+      </c>
+      <c r="H227" s="8">
+        <v>0</v>
+      </c>
+      <c r="I227" s="8">
+        <v>0</v>
+      </c>
+      <c r="J227" s="8">
+        <v>1430</v>
+      </c>
+      <c r="K227" t="str">
+        <f t="shared" si="17"/>
+        <v>Yes</v>
+      </c>
+      <c r="L227" t="str">
+        <f t="shared" si="18"/>
+        <v>No</v>
+      </c>
+      <c r="M227" t="str">
+        <f t="shared" si="19"/>
+        <v>No</v>
+      </c>
+      <c r="N227" t="str">
+        <f t="shared" si="20"/>
+        <v>Yes</v>
+      </c>
+      <c r="O227" t="str">
+        <f t="shared" si="16"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="228" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A228" s="1">
+        <v>43205</v>
+      </c>
+      <c r="B228" s="8">
+        <v>2822</v>
+      </c>
+      <c r="C228" s="8">
+        <v>6278</v>
+      </c>
+      <c r="D228" s="8">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="E228" s="8">
+        <v>13</v>
+      </c>
+      <c r="F228" s="8">
+        <v>806</v>
+      </c>
+      <c r="G228" s="8">
+        <v>259</v>
+      </c>
+      <c r="H228" s="8">
+        <v>0</v>
+      </c>
+      <c r="I228" s="8">
+        <v>0</v>
+      </c>
+      <c r="J228" s="8">
+        <v>1090</v>
+      </c>
+      <c r="K228" t="str">
+        <f t="shared" si="17"/>
+        <v>No</v>
+      </c>
+      <c r="L228" t="str">
+        <f t="shared" si="18"/>
+        <v>No</v>
+      </c>
+      <c r="M228" t="str">
+        <f t="shared" si="19"/>
+        <v>No</v>
+      </c>
+      <c r="N228" t="str">
+        <f t="shared" si="20"/>
+        <v>Yes</v>
+      </c>
+      <c r="O228" t="str">
+        <f t="shared" si="16"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="229" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A229" s="1">
+        <v>43206</v>
+      </c>
+      <c r="B229" s="8">
+        <v>3871</v>
+      </c>
+      <c r="C229" s="8">
+        <v>11645</v>
+      </c>
+      <c r="D229" s="8">
+        <v>8.67</v>
+      </c>
+      <c r="E229" s="8">
+        <v>11</v>
+      </c>
+      <c r="F229" s="8">
+        <v>688</v>
+      </c>
+      <c r="G229" s="8">
+        <v>315</v>
+      </c>
+      <c r="H229" s="8">
+        <v>6</v>
+      </c>
+      <c r="I229" s="8">
+        <v>50</v>
+      </c>
+      <c r="J229" s="8">
+        <v>2188</v>
+      </c>
+      <c r="K229" t="str">
+        <f t="shared" si="17"/>
+        <v>Yes</v>
+      </c>
+      <c r="L229" t="str">
+        <f t="shared" si="18"/>
+        <v>Yes</v>
+      </c>
+      <c r="M229" t="str">
+        <f t="shared" si="19"/>
+        <v>Yes</v>
+      </c>
+      <c r="N229" t="str">
+        <f t="shared" si="20"/>
+        <v>No</v>
+      </c>
+      <c r="O229" t="str">
+        <f t="shared" si="16"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="230" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A230" s="1">
+        <v>43207</v>
+      </c>
+      <c r="B230" s="8">
+        <v>3468</v>
+      </c>
+      <c r="C230" s="8">
+        <v>8667</v>
+      </c>
+      <c r="D230" s="8">
+        <v>6.55</v>
+      </c>
+      <c r="E230" s="8">
+        <v>16</v>
+      </c>
+      <c r="F230" s="8">
+        <v>800</v>
+      </c>
+      <c r="G230" s="8">
+        <v>200</v>
+      </c>
+      <c r="H230" s="8">
+        <v>24</v>
+      </c>
+      <c r="I230" s="8">
+        <v>47</v>
+      </c>
+      <c r="J230" s="8">
+        <v>1640</v>
+      </c>
+      <c r="K230" t="str">
+        <f t="shared" si="17"/>
+        <v>Yes</v>
+      </c>
+      <c r="L230" t="str">
+        <f t="shared" si="18"/>
+        <v>Yes</v>
+      </c>
+      <c r="M230" t="str">
+        <f t="shared" si="19"/>
+        <v>Yes</v>
+      </c>
+      <c r="N230" t="str">
+        <f t="shared" si="20"/>
+        <v>No</v>
+      </c>
+      <c r="O230" t="str">
+        <f t="shared" si="16"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="231" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A231" s="1">
+        <v>43208</v>
+      </c>
+      <c r="B231" s="8">
+        <v>3549</v>
+      </c>
+      <c r="C231" s="8">
+        <v>11007</v>
+      </c>
+      <c r="D231" s="8">
+        <v>8.59</v>
+      </c>
+      <c r="E231" s="8">
+        <v>30</v>
+      </c>
+      <c r="F231" s="8">
+        <v>683</v>
+      </c>
+      <c r="G231" s="8">
+        <v>336</v>
+      </c>
+      <c r="H231" s="8">
+        <v>16</v>
+      </c>
+      <c r="I231" s="8">
+        <v>26</v>
+      </c>
+      <c r="J231" s="8">
+        <v>1952</v>
+      </c>
+      <c r="K231" t="str">
+        <f t="shared" si="17"/>
+        <v>Yes</v>
+      </c>
+      <c r="L231" t="str">
+        <f t="shared" si="18"/>
+        <v>Yes</v>
+      </c>
+      <c r="M231" t="str">
+        <f t="shared" si="19"/>
+        <v>No</v>
+      </c>
+      <c r="N231" t="str">
+        <f t="shared" si="20"/>
+        <v>No</v>
+      </c>
+      <c r="O231" t="str">
+        <f t="shared" si="16"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="232" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A232" s="1">
+        <v>43209</v>
+      </c>
+      <c r="B232" s="8">
+        <v>3560</v>
+      </c>
+      <c r="C232" s="8">
+        <v>10258</v>
+      </c>
+      <c r="D232" s="8">
+        <v>7.76</v>
+      </c>
+      <c r="E232" s="8">
+        <v>19</v>
+      </c>
+      <c r="F232" s="8">
+        <v>681</v>
+      </c>
+      <c r="G232" s="8">
+        <v>260</v>
+      </c>
+      <c r="H232" s="8">
+        <v>22</v>
+      </c>
+      <c r="I232" s="8">
+        <v>47</v>
+      </c>
+      <c r="J232" s="8">
+        <v>1895</v>
+      </c>
+      <c r="K232" t="str">
+        <f t="shared" si="17"/>
+        <v>Yes</v>
+      </c>
+      <c r="L232" t="str">
+        <f t="shared" si="18"/>
+        <v>Yes</v>
+      </c>
+      <c r="M232" t="str">
+        <f t="shared" si="19"/>
+        <v>Yes</v>
+      </c>
+      <c r="N232" t="str">
+        <f t="shared" si="20"/>
+        <v>No</v>
+      </c>
+      <c r="O232" t="str">
+        <f t="shared" si="16"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="233" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A233" s="1">
+        <v>43210</v>
+      </c>
+      <c r="B233" s="8">
+        <v>3420</v>
+      </c>
+      <c r="C233" s="8">
+        <v>10856</v>
+      </c>
+      <c r="D233" s="8">
+        <v>8.33</v>
+      </c>
+      <c r="E233" s="8">
+        <v>28</v>
+      </c>
+      <c r="F233" s="8">
+        <v>684</v>
+      </c>
+      <c r="G233" s="8">
+        <v>278</v>
+      </c>
+      <c r="H233" s="8">
+        <v>28</v>
+      </c>
+      <c r="I233" s="8">
+        <v>23</v>
+      </c>
+      <c r="J233" s="8">
+        <v>1752</v>
+      </c>
+      <c r="K233" t="str">
+        <f t="shared" si="17"/>
+        <v>Yes</v>
+      </c>
+      <c r="L233" t="str">
+        <f t="shared" si="18"/>
+        <v>Yes</v>
+      </c>
+      <c r="M233" t="str">
+        <f t="shared" si="19"/>
+        <v>No</v>
+      </c>
+      <c r="N233" t="str">
+        <f t="shared" si="20"/>
+        <v>No</v>
+      </c>
+      <c r="O233" t="str">
+        <f t="shared" si="16"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="234" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A234" s="1">
+        <v>43211</v>
+      </c>
+      <c r="B234" s="8">
+        <v>3625</v>
+      </c>
+      <c r="C234" s="8">
+        <v>9681</v>
+      </c>
+      <c r="D234" s="8">
+        <v>7.2</v>
+      </c>
+      <c r="E234" s="8">
+        <v>8</v>
+      </c>
+      <c r="F234" s="8">
+        <v>673</v>
+      </c>
+      <c r="G234" s="8">
+        <v>154</v>
+      </c>
+      <c r="H234" s="8">
+        <v>25</v>
+      </c>
+      <c r="I234" s="8">
+        <v>79</v>
+      </c>
+      <c r="J234" s="8">
+        <v>1873</v>
+      </c>
+      <c r="K234" t="str">
+        <f t="shared" si="17"/>
+        <v>Yes</v>
+      </c>
+      <c r="L234" t="str">
+        <f t="shared" si="18"/>
+        <v>Yes</v>
+      </c>
+      <c r="M234" t="str">
+        <f t="shared" si="19"/>
+        <v>Yes</v>
+      </c>
+      <c r="N234" t="str">
+        <f t="shared" si="20"/>
+        <v>No</v>
+      </c>
+      <c r="O234" t="str">
+        <f t="shared" si="16"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="235" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A235" s="1">
+        <v>43212</v>
+      </c>
+      <c r="B235" s="8">
+        <v>2876</v>
+      </c>
+      <c r="C235" s="8">
+        <v>7091</v>
+      </c>
+      <c r="D235" s="8">
+        <v>5.53</v>
+      </c>
+      <c r="E235" s="8">
+        <v>12</v>
+      </c>
+      <c r="F235" s="8">
+        <v>710</v>
+      </c>
+      <c r="G235" s="8">
+        <v>254</v>
+      </c>
+      <c r="H235" s="8">
+        <v>5</v>
+      </c>
+      <c r="I235" s="8">
+        <v>2</v>
+      </c>
+      <c r="J235" s="8">
+        <v>1160</v>
+      </c>
+      <c r="K235" t="str">
+        <f t="shared" si="17"/>
+        <v>No</v>
+      </c>
+      <c r="L235" t="str">
+        <f t="shared" si="18"/>
+        <v>No</v>
+      </c>
+      <c r="M235" t="str">
+        <f t="shared" si="19"/>
+        <v>No</v>
+      </c>
+      <c r="N235" t="str">
+        <f t="shared" si="20"/>
+        <v>Yes</v>
+      </c>
+      <c r="O235" t="str">
+        <f t="shared" si="16"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="236" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A236" s="1">
+        <v>43213</v>
+      </c>
+      <c r="B236" s="8">
+        <v>3673</v>
+      </c>
+      <c r="C236" s="8">
+        <v>9868</v>
+      </c>
+      <c r="D236" s="8">
+        <v>7.52</v>
+      </c>
+      <c r="E236" s="8">
+        <v>16</v>
+      </c>
+      <c r="F236" s="8">
+        <v>722</v>
+      </c>
+      <c r="G236" s="8">
+        <v>189</v>
+      </c>
+      <c r="H236" s="8">
+        <v>21</v>
+      </c>
+      <c r="I236" s="8">
+        <v>75</v>
+      </c>
+      <c r="J236" s="8">
+        <v>1928</v>
+      </c>
+      <c r="K236" t="str">
+        <f t="shared" si="17"/>
+        <v>Yes</v>
+      </c>
+      <c r="L236" t="str">
+        <f t="shared" si="18"/>
+        <v>Yes</v>
+      </c>
+      <c r="M236" t="str">
+        <f t="shared" si="19"/>
+        <v>Yes</v>
+      </c>
+      <c r="N236" t="str">
+        <f t="shared" si="20"/>
+        <v>No</v>
+      </c>
+      <c r="O236" t="str">
+        <f t="shared" si="16"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="237" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A237" s="1">
+        <v>43214</v>
+      </c>
+      <c r="B237" s="8">
+        <v>2971</v>
+      </c>
+      <c r="C237" s="8">
+        <v>6821</v>
+      </c>
+      <c r="D237" s="8">
+        <v>5.32</v>
+      </c>
+      <c r="E237" s="8">
+        <v>10</v>
+      </c>
+      <c r="F237" s="8">
+        <v>773</v>
+      </c>
+      <c r="G237" s="8">
+        <v>196</v>
+      </c>
+      <c r="H237" s="8">
+        <v>4</v>
+      </c>
+      <c r="I237" s="8">
+        <v>20</v>
+      </c>
+      <c r="J237" s="8">
+        <v>1095</v>
+      </c>
+      <c r="K237" t="str">
+        <f t="shared" si="17"/>
+        <v>No</v>
+      </c>
+      <c r="L237" t="str">
+        <f t="shared" si="18"/>
+        <v>No</v>
+      </c>
+      <c r="M237" t="str">
+        <f t="shared" si="19"/>
+        <v>No</v>
+      </c>
+      <c r="N237" t="str">
+        <f t="shared" si="20"/>
+        <v>Yes</v>
+      </c>
+      <c r="O237" t="str">
+        <f t="shared" si="16"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="238" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A238" s="1">
+        <v>43215</v>
+      </c>
+      <c r="B238" s="8">
+        <v>3020</v>
+      </c>
+      <c r="C238" s="8">
+        <v>6183</v>
+      </c>
+      <c r="D238" s="8">
+        <v>4.7</v>
+      </c>
+      <c r="E238" s="8">
+        <v>7</v>
+      </c>
+      <c r="F238" s="8">
+        <v>681</v>
+      </c>
+      <c r="G238" s="8">
+        <v>169</v>
+      </c>
+      <c r="H238" s="8">
+        <v>26</v>
+      </c>
+      <c r="I238" s="8">
+        <v>7</v>
+      </c>
+      <c r="J238" s="8">
+        <v>1113</v>
+      </c>
+      <c r="K238" t="str">
+        <f t="shared" si="17"/>
+        <v>No</v>
+      </c>
+      <c r="L238" t="str">
+        <f t="shared" si="18"/>
+        <v>No</v>
+      </c>
+      <c r="M238" t="str">
+        <f t="shared" si="19"/>
+        <v>No</v>
+      </c>
+      <c r="N238" t="str">
+        <f t="shared" si="20"/>
+        <v>No</v>
+      </c>
+      <c r="O238" t="str">
+        <f t="shared" ref="O238:O243" si="21">IF(D238&gt;5,"Yes","No")</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="239" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A239" s="1">
+        <v>43216</v>
+      </c>
+      <c r="B239" s="8">
+        <v>3555</v>
+      </c>
+      <c r="C239" s="8">
+        <v>9294</v>
+      </c>
+      <c r="D239" s="8">
+        <v>6.89</v>
+      </c>
+      <c r="E239" s="8">
+        <v>10</v>
+      </c>
+      <c r="F239" s="8">
+        <v>734</v>
+      </c>
+      <c r="G239" s="8">
+        <v>211</v>
+      </c>
+      <c r="H239" s="8">
+        <v>23</v>
+      </c>
+      <c r="I239" s="8">
+        <v>48</v>
+      </c>
+      <c r="J239" s="8">
+        <v>1741</v>
+      </c>
+      <c r="K239" t="str">
+        <f t="shared" si="17"/>
+        <v>Yes</v>
+      </c>
+      <c r="L239" t="str">
+        <f t="shared" si="18"/>
+        <v>Yes</v>
+      </c>
+      <c r="M239" t="str">
+        <f t="shared" si="19"/>
+        <v>Yes</v>
+      </c>
+      <c r="N239" t="str">
+        <f t="shared" si="20"/>
+        <v>No</v>
+      </c>
+      <c r="O239" t="str">
+        <f t="shared" si="21"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="240" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A240" s="1">
+        <v>43217</v>
+      </c>
+      <c r="B240" s="8">
+        <v>2846</v>
+      </c>
+      <c r="C240" s="8">
+        <v>7313</v>
+      </c>
+      <c r="D240" s="8">
+        <v>5.7</v>
+      </c>
+      <c r="E240" s="8">
+        <v>16</v>
+      </c>
+      <c r="F240" s="8">
+        <v>807</v>
+      </c>
+      <c r="G240" s="8">
+        <v>212</v>
+      </c>
+      <c r="H240" s="8">
+        <v>5</v>
+      </c>
+      <c r="I240" s="8">
+        <v>4</v>
+      </c>
+      <c r="J240" s="8">
+        <v>1051</v>
+      </c>
+      <c r="K240" t="str">
+        <f t="shared" si="17"/>
+        <v>No</v>
+      </c>
+      <c r="L240" t="str">
+        <f t="shared" si="18"/>
+        <v>No</v>
+      </c>
+      <c r="M240" t="str">
+        <f t="shared" si="19"/>
+        <v>No</v>
+      </c>
+      <c r="N240" t="str">
+        <f t="shared" si="20"/>
+        <v>Yes</v>
+      </c>
+      <c r="O240" t="str">
+        <f t="shared" si="21"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="241" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A241" s="1">
+        <v>43218</v>
+      </c>
+      <c r="B241" s="8">
+        <v>2919</v>
+      </c>
+      <c r="C241" s="8">
+        <v>6986</v>
+      </c>
+      <c r="D241" s="8">
+        <v>5.45</v>
+      </c>
+      <c r="E241" s="8">
+        <v>33</v>
+      </c>
+      <c r="F241" s="8">
+        <v>824</v>
+      </c>
+      <c r="G241" s="8">
+        <v>245</v>
+      </c>
+      <c r="H241" s="8">
+        <v>0</v>
+      </c>
+      <c r="I241" s="8">
+        <v>0</v>
+      </c>
+      <c r="J241" s="8">
+        <v>1149</v>
+      </c>
+      <c r="K241" t="str">
+        <f t="shared" si="17"/>
+        <v>No</v>
+      </c>
+      <c r="L241" t="str">
+        <f t="shared" si="18"/>
+        <v>No</v>
+      </c>
+      <c r="M241" t="str">
+        <f t="shared" si="19"/>
+        <v>No</v>
+      </c>
+      <c r="N241" t="str">
+        <f t="shared" si="20"/>
+        <v>Yes</v>
+      </c>
+      <c r="O241" t="str">
+        <f t="shared" si="21"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="242" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A242" s="1">
+        <v>43219</v>
+      </c>
+      <c r="B242" s="8">
+        <v>3402</v>
+      </c>
+      <c r="C242" s="8">
+        <v>8474</v>
+      </c>
+      <c r="D242" s="8">
+        <v>6.2</v>
+      </c>
+      <c r="E242" s="8">
+        <v>15</v>
+      </c>
+      <c r="F242" s="8">
+        <v>713</v>
+      </c>
+      <c r="G242" s="8">
+        <v>166</v>
+      </c>
+      <c r="H242" s="8">
+        <v>36</v>
+      </c>
+      <c r="I242" s="8">
+        <v>55</v>
+      </c>
+      <c r="J242" s="8">
+        <v>1611</v>
+      </c>
+      <c r="K242" t="str">
+        <f t="shared" si="17"/>
+        <v>Yes</v>
+      </c>
+      <c r="L242" t="str">
+        <f t="shared" si="18"/>
+        <v>Yes</v>
+      </c>
+      <c r="M242" t="str">
+        <f t="shared" si="19"/>
+        <v>Yes</v>
+      </c>
+      <c r="N242" t="str">
+        <f t="shared" si="20"/>
+        <v>No</v>
+      </c>
+      <c r="O242" t="str">
+        <f t="shared" si="21"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="243" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A243" s="1">
+        <v>43220</v>
+      </c>
+      <c r="B243" s="8">
+        <v>3597</v>
+      </c>
+      <c r="C243" s="8">
+        <v>8258</v>
+      </c>
+      <c r="D243" s="8">
+        <v>6.14</v>
+      </c>
+      <c r="E243" s="8">
+        <v>14</v>
+      </c>
+      <c r="F243" s="8">
+        <v>712</v>
+      </c>
+      <c r="G243" s="8">
+        <v>238</v>
+      </c>
+      <c r="H243" s="8">
+        <v>18</v>
+      </c>
+      <c r="I243" s="8">
+        <v>55</v>
+      </c>
+      <c r="J243" s="8">
+        <v>1863</v>
+      </c>
+      <c r="K243" t="str">
+        <f t="shared" si="17"/>
+        <v>Yes</v>
+      </c>
+      <c r="L243" t="str">
+        <f t="shared" si="18"/>
+        <v>Yes</v>
+      </c>
+      <c r="M243" t="str">
+        <f t="shared" si="19"/>
+        <v>Yes</v>
+      </c>
+      <c r="N243" t="str">
+        <f t="shared" si="20"/>
+        <v>No</v>
+      </c>
+      <c r="O243" t="str">
+        <f t="shared" si="21"/>
         <v>Yes</v>
       </c>
     </row>

</xml_diff>